<commit_message>
Mise a jour de l'excel suivi projet
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samle\OneDrive\Documents\Univ\travail\S4\MAP401\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univgrenoble-my.sharepoint.com/personal/lepins_azure_univ-grenoble-alpes_fr/Documents/S4/MAP401/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA664407-DAAF-4DC6-8B3F-AA20820C83C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{EA664407-DAAF-4DC6-8B3F-AA20820C83C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8611DC4-3CB2-452C-B451-D3B69A8E2A38}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiagrammeGanttReel" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="JournalDeBord_Exemple" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t>s3</t>
   </si>
@@ -375,9 +376,6 @@
     <t xml:space="preserve">Mise en place de l'image de marque </t>
   </si>
   <si>
-    <t xml:space="preserve">En cours </t>
-  </si>
-  <si>
     <t xml:space="preserve">mettre à jour l'image de marque apres chaque contour  </t>
   </si>
   <si>
@@ -394,9 +392,6 @@
  déjà pour l'image de marque </t>
   </si>
   <si>
-    <t xml:space="preserve">Non commencer </t>
-  </si>
-  <si>
     <t>TACHE 5 Partie 2</t>
   </si>
   <si>
@@ -406,10 +401,10 @@
     <t xml:space="preserve">ecrire un programme qui lit une image dans un fichier PBM et cree un fichier EPS </t>
   </si>
   <si>
-    <t>il devra aussi ecrire le nombre de contours de l'image ainsi que de segments ( eventuellement points)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mise en place d'une fonction qui met l'ensemble des coutours dans un fichier </t>
+  </si>
+  <si>
+    <t xml:space="preserve">il devra aussi ecrire le nombre de contours de l'image ainsi que de segments </t>
   </si>
 </sst>
 </file>
@@ -489,7 +484,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -517,18 +512,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -816,7 +799,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -874,6 +857,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,21 +875,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="En-tête" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -916,8 +893,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFFF9900"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -929,6 +906,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1318,8 +1299,8 @@
   </sheetPr>
   <dimension ref="A2:AJ15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1339,74 +1320,74 @@
     <row r="3" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="37" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="35" t="s">
+      <c r="J3" s="40"/>
+      <c r="K3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="37" t="s">
+      <c r="L3" s="38"/>
+      <c r="M3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="35" t="s">
+      <c r="N3" s="40"/>
+      <c r="O3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35" t="s">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35" t="s">
+      <c r="R3" s="38"/>
+      <c r="S3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="35"/>
-      <c r="U3" s="37" t="s">
+      <c r="T3" s="38"/>
+      <c r="U3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="37"/>
-      <c r="W3" s="35" t="s">
+      <c r="V3" s="40"/>
+      <c r="W3" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="37" t="s">
+      <c r="X3" s="38"/>
+      <c r="Y3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="35" t="s">
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="37" t="s">
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37" t="s">
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37" t="s">
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37" t="s">
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="AJ3" s="37"/>
+      <c r="AJ3" s="40"/>
     </row>
     <row r="4" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
@@ -1423,30 +1404,30 @@
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="41"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="38" t="s">
+      <c r="S4" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="38"/>
+      <c r="T4" s="41"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="38" t="s">
+      <c r="AA4" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="38"/>
+      <c r="AB4" s="41"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -1471,24 +1452,24 @@
       <c r="H5" s="19"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
+      <c r="AA5" s="41"/>
+      <c r="AB5" s="41"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -1511,26 +1492,26 @@
       <c r="F6" s="21"/>
       <c r="G6" s="23"/>
       <c r="H6" s="24"/>
-      <c r="I6" s="40"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="2"/>
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="38"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -1553,26 +1534,26 @@
       <c r="F7" s="5"/>
       <c r="G7" s="17"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="45"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="37"/>
       <c r="N7" s="19"/>
-      <c r="O7" s="45"/>
+      <c r="O7" s="37"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
       <c r="U7" s="2"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="5"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -1586,7 +1567,7 @@
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="2"/>
@@ -1596,24 +1577,24 @@
       <c r="G8" s="2"/>
       <c r="H8" s="5"/>
       <c r="I8" s="17"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="5"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="19"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
       <c r="U8" s="2"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="5"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -1623,11 +1604,11 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="5"/>
     </row>
-    <row r="9" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="44" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="2"/>
@@ -1638,24 +1619,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="20"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
       <c r="M9" s="17"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="2"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="6"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
       <c r="U9" s="2"/>
       <c r="V9" s="5"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="5"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="5"/>
       <c r="AE9" s="2"/>
@@ -1680,24 +1661,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="5"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
       <c r="U10" s="2"/>
       <c r="V10" s="5"/>
       <c r="W10" s="2"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="5"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="2"/>
@@ -1722,24 +1703,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="5"/>
       <c r="AE11" s="2"/>
@@ -1764,24 +1745,24 @@
       <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="2"/>
       <c r="N12" s="5"/>
       <c r="O12" s="2"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
       <c r="U12" s="2"/>
       <c r="V12" s="5"/>
       <c r="W12" s="2"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="5"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
+      <c r="AA12" s="41"/>
+      <c r="AB12" s="41"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="2"/>
@@ -1806,24 +1787,24 @@
       <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="38"/>
-      <c r="AB13" s="38"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="2"/>
@@ -1846,24 +1827,24 @@
       <c r="H14" s="5"/>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
       <c r="U14" s="2"/>
       <c r="V14" s="5"/>
       <c r="W14" s="2"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="5"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="38"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="2"/>
@@ -1911,8 +1892,8 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A31" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2487,7 +2468,7 @@
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
@@ -2530,16 +2511,19 @@
         <v>44964</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="30">
         <v>44978</v>
       </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="52" t="str">
-        <f>G31</f>
-        <v xml:space="preserve">Non commencer </v>
+      <c r="F28" s="30">
+        <f>E28</f>
+        <v>44978</v>
+      </c>
+      <c r="G28" s="33" t="str">
+        <f>G27</f>
+        <v>terminer</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -2552,17 +2536,20 @@
         <v>44964</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="30">
         <f>E28</f>
         <v>44978</v>
       </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="49" t="str">
-        <f>G30</f>
-        <v xml:space="preserve">En cours </v>
+      <c r="F29" s="30">
+        <f>E29</f>
+        <v>44978</v>
+      </c>
+      <c r="G29" s="33" t="str">
+        <f>G28</f>
+        <v>terminer</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="48.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2575,18 +2562,22 @@
         <v>44964</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" s="30">
         <f>E29</f>
         <v>44978</v>
       </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="48" t="s">
-        <v>87</v>
+      <c r="F30" s="30">
+        <f>E30</f>
+        <v>44978</v>
+      </c>
+      <c r="G30" s="33" t="str">
+        <f>G29</f>
+        <v>terminer</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -2599,23 +2590,27 @@
         <v>44964</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="30">
         <f>E30</f>
         <v>44978</v>
       </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="50" t="s">
-        <v>93</v>
+      <c r="F31" s="30">
+        <f>E31</f>
+        <v>44978</v>
+      </c>
+      <c r="G31" s="33" t="str">
+        <f>G30</f>
+        <v>terminer</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
@@ -2627,19 +2622,25 @@
         <f>A31+1</f>
         <v>25</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="51" t="s">
-        <v>95</v>
+      <c r="B33" s="30">
+        <f>E28</f>
+        <v>44978</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>93</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="30">
         <f>E31</f>
         <v>44978</v>
       </c>
-      <c r="F33" s="29"/>
-      <c r="G33" s="50" t="str">
-        <f>G31</f>
-        <v xml:space="preserve">Non commencer </v>
+      <c r="F33" s="30">
+        <f>E33</f>
+        <v>44978</v>
+      </c>
+      <c r="G33" s="33" t="str">
+        <f>G30</f>
+        <v>terminer</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -2647,19 +2648,25 @@
         <f>A33+1</f>
         <v>26</v>
       </c>
-      <c r="B34" s="29"/>
-      <c r="C34" s="51" t="s">
-        <v>96</v>
+      <c r="B34" s="30">
+        <f>B33</f>
+        <v>44978</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>94</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="30">
         <f>E33</f>
         <v>44978</v>
       </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="50" t="str">
+      <c r="F34" s="30">
+        <f>E34</f>
+        <v>44978</v>
+      </c>
+      <c r="G34" s="32" t="str">
         <f>G33</f>
-        <v xml:space="preserve">Non commencer </v>
+        <v>terminer</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,19 +2674,25 @@
         <f>A34+1</f>
         <v>27</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="51" t="s">
-        <v>97</v>
+      <c r="B35" s="30">
+        <f>B34</f>
+        <v>44978</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>96</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="30">
         <f>E34</f>
         <v>44978</v>
       </c>
-      <c r="F35" s="29"/>
-      <c r="G35" s="50" t="str">
+      <c r="F35" s="30">
+        <f>E35</f>
+        <v>44978</v>
+      </c>
+      <c r="G35" s="32" t="str">
         <f>G34</f>
-        <v xml:space="preserve">Non commencer </v>
+        <v>terminer</v>
       </c>
     </row>
   </sheetData>
@@ -2711,74 +2724,74 @@
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="35" t="s">
+      <c r="F3" s="42"/>
+      <c r="G3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="37" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37" t="s">
+      <c r="J3" s="40"/>
+      <c r="K3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="35" t="s">
+      <c r="L3" s="40"/>
+      <c r="M3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35" t="s">
+      <c r="N3" s="38"/>
+      <c r="O3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35" t="s">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35" t="s">
+      <c r="R3" s="38"/>
+      <c r="S3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="35"/>
-      <c r="U3" s="37" t="s">
+      <c r="T3" s="38"/>
+      <c r="U3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="37"/>
-      <c r="W3" s="35" t="s">
+      <c r="V3" s="40"/>
+      <c r="W3" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="37" t="s">
+      <c r="X3" s="38"/>
+      <c r="Y3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="35" t="s">
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="37" t="s">
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37" t="s">
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37" t="s">
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37" t="s">
+      <c r="AH3" s="40"/>
+      <c r="AI3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="AJ3" s="37"/>
+      <c r="AJ3" s="40"/>
     </row>
     <row r="4" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -2795,30 +2808,30 @@
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="41"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="38" t="s">
+      <c r="S4" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="38"/>
+      <c r="T4" s="41"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-      <c r="AA4" s="38" t="s">
+      <c r="AA4" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="38"/>
+      <c r="AB4" s="41"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -2843,24 +2856,24 @@
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="38"/>
+      <c r="AA5" s="41"/>
+      <c r="AB5" s="41"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -2885,24 +2898,24 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
       <c r="M6" s="2"/>
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="38"/>
-      <c r="T6" s="38"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="38"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -2927,24 +2940,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
       <c r="M7" s="2"/>
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
       <c r="U7" s="2"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="38"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -2969,24 +2982,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
       <c r="M8" s="9"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="38"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
       <c r="U8" s="2"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="38"/>
+      <c r="AA8" s="41"/>
+      <c r="AB8" s="41"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -3011,24 +3024,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="38"/>
-      <c r="T9" s="38"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
       <c r="U9" s="13"/>
       <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
+      <c r="AA9" s="41"/>
+      <c r="AB9" s="41"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="5"/>
       <c r="AE9" s="2"/>
@@ -3053,24 +3066,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="38"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
       <c r="U10" s="2"/>
       <c r="V10" s="5"/>
       <c r="W10" s="9"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="11"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
+      <c r="AA10" s="41"/>
+      <c r="AB10" s="41"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="2"/>
@@ -3095,24 +3108,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="11"/>
       <c r="AE11" s="2"/>
@@ -3135,24 +3148,24 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="13"/>
       <c r="N12" s="12"/>
       <c r="O12" s="13"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="38"/>
-      <c r="T12" s="38"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
       <c r="U12" s="13"/>
       <c r="V12" s="10"/>
       <c r="W12" s="13"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="38"/>
+      <c r="AA12" s="41"/>
+      <c r="AB12" s="41"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="2"/>
@@ -3175,24 +3188,24 @@
       <c r="H13" s="6"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-      <c r="AA13" s="38"/>
-      <c r="AB13" s="38"/>
+      <c r="AA13" s="41"/>
+      <c r="AB13" s="41"/>
       <c r="AC13" s="9"/>
       <c r="AD13" s="11"/>
       <c r="AE13" s="2"/>
@@ -3215,24 +3228,24 @@
       <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="38"/>
-      <c r="T14" s="38"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
       <c r="U14" s="2"/>
       <c r="V14" s="5"/>
       <c r="W14" s="2"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="38"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="9"/>

</xml_diff>

<commit_message>
end week 13 , change Excel and tache7
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samle\VSC-Rpertoire\MAP401\bitmap-vectoriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1EEB931-1C08-4D55-8CB7-AE8968CC0A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490718E6-77E4-4E6A-A50C-05C956EAAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiagrammeGanttReel" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="JournalDeBord_Exemple" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
   <si>
     <t>s3</t>
   </si>
@@ -464,6 +463,44 @@
 Blanc</t>
     </r>
   </si>
+  <si>
+    <t>TACHE 7 Partie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mettre en place le type bezierr2 et 3 , calcule pointC(t), pour une courbe de degre 2 et 3
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La conversion de bezier de degre 2 à degreé 3 </t>
+  </si>
+  <si>
+    <t>ecrire approx_bezizer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tester les deux cas </t>
+  </si>
+  <si>
+    <t>implementer l'algo de douglas peucker pour un degré 2</t>
+  </si>
+  <si>
+    <t>ajoue sortie EPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecrire le programme main pour ces fonctions </t>
+  </si>
+  <si>
+    <t>Commencer</t>
+  </si>
+  <si>
+    <t>Non Commencer</t>
+  </si>
+  <si>
+    <t>TACHE 7 Partie 2 
+(Objectif de bien la commencer avant les vancances )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire pareil que au-dessus mais pour une courbe de bezier de degré 3 </t>
+  </si>
 </sst>
 </file>
 
@@ -548,7 +585,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,8 +628,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -875,19 +918,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="hair">
         <color indexed="8"/>
@@ -908,6 +938,26 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -925,7 +975,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1009,19 +1059,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1030,8 +1073,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="En-tête" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1446,8 +1511,8 @@
   </sheetPr>
   <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1467,74 +1532,74 @@
     <row r="2" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="53" t="s">
+      <c r="H2" s="52"/>
+      <c r="I2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="55" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="55"/>
-      <c r="M2" s="53" t="s">
+      <c r="L2" s="52"/>
+      <c r="M2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="53"/>
-      <c r="O2" s="55" t="s">
+      <c r="N2" s="54"/>
+      <c r="O2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55" t="s">
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55" t="s">
+      <c r="R2" s="52"/>
+      <c r="S2" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53" t="s">
+      <c r="T2" s="52"/>
+      <c r="U2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="53"/>
-      <c r="W2" s="55" t="s">
+      <c r="V2" s="54"/>
+      <c r="W2" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="53" t="s">
+      <c r="X2" s="52"/>
+      <c r="Y2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="55" t="s">
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="53" t="s">
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53" t="s">
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53" t="s">
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53" t="s">
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="53"/>
+      <c r="AJ2" s="54"/>
     </row>
     <row r="3" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1551,30 +1616,30 @@
       <c r="H3" s="5"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="54"/>
+      <c r="L3" s="55"/>
       <c r="M3" s="2"/>
       <c r="N3" s="5"/>
       <c r="O3" s="2"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="54" t="s">
+      <c r="S3" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="54"/>
+      <c r="T3" s="55"/>
       <c r="U3" s="2"/>
       <c r="V3" s="5"/>
       <c r="W3" s="2"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="54" t="s">
+      <c r="AA3" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="54"/>
+      <c r="AB3" s="55"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="2"/>
@@ -1599,24 +1664,24 @@
       <c r="H4" s="19"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="54"/>
+      <c r="AA4" s="55"/>
+      <c r="AB4" s="55"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -1641,24 +1706,24 @@
       <c r="H5" s="24"/>
       <c r="I5" s="27"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="55"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -1683,24 +1748,24 @@
       <c r="H6" s="21"/>
       <c r="I6" s="28"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
       <c r="M6" s="29"/>
       <c r="N6" s="19"/>
       <c r="O6" s="29"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="54"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="55"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -1725,23 +1790,23 @@
       <c r="H7" s="5"/>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
       <c r="M7" s="23"/>
       <c r="N7" s="30"/>
       <c r="O7" s="19"/>
       <c r="Q7" s="29"/>
       <c r="R7" s="19"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
       <c r="U7" s="29"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="5"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="19"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="5"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="54"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="55"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -1766,24 +1831,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
       <c r="M8" s="17"/>
       <c r="N8" s="21"/>
       <c r="O8" s="31"/>
       <c r="P8" s="44"/>
       <c r="Q8" s="45"/>
       <c r="R8" s="46"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="29"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="22"/>
       <c r="Z8" s="19"/>
-      <c r="AA8" s="54"/>
-      <c r="AB8" s="54"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="55"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -1808,24 +1873,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="17"/>
       <c r="P9" s="20"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="20"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="64"/>
+      <c r="X9" s="64"/>
       <c r="Y9" s="44"/>
       <c r="Z9" s="32"/>
-      <c r="AA9" s="54"/>
-      <c r="AB9" s="54"/>
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="55"/>
       <c r="AC9" s="29"/>
       <c r="AD9" s="19"/>
       <c r="AE9" s="29"/>
@@ -1839,7 +1904,7 @@
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2"/>
@@ -1850,28 +1915,28 @@
       <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="54"/>
-      <c r="T10" s="54"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
       <c r="U10" s="17"/>
       <c r="V10" s="20"/>
       <c r="W10" s="17"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="17"/>
       <c r="Z10" s="20"/>
-      <c r="AA10" s="54"/>
-      <c r="AB10" s="54"/>
-      <c r="AC10" s="48"/>
-      <c r="AD10" s="49"/>
-      <c r="AE10" s="50"/>
-      <c r="AF10" s="51"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="55"/>
+      <c r="AC10" s="47"/>
+      <c r="AD10" s="48"/>
+      <c r="AE10" s="49"/>
+      <c r="AF10" s="50"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="5"/>
       <c r="AI10" s="2"/>
@@ -1881,7 +1946,7 @@
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2"/>
@@ -1892,28 +1957,28 @@
       <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="55"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="54"/>
-      <c r="AB11" s="54"/>
-      <c r="AC11" s="48"/>
-      <c r="AD11" s="49"/>
-      <c r="AE11" s="50"/>
-      <c r="AF11" s="51"/>
+      <c r="AA11" s="55"/>
+      <c r="AB11" s="55"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="48"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="50"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="5"/>
       <c r="AI11" s="2"/>
@@ -1934,24 +1999,24 @@
       <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
       <c r="M12" s="2"/>
       <c r="N12" s="5"/>
       <c r="O12" s="2"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="54"/>
-      <c r="T12" s="54"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="55"/>
       <c r="U12" s="2"/>
       <c r="V12" s="5"/>
       <c r="W12" s="2"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="5"/>
-      <c r="AA12" s="54"/>
-      <c r="AB12" s="54"/>
+      <c r="AA12" s="55"/>
+      <c r="AB12" s="55"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="20"/>
       <c r="AE12" s="17"/>
@@ -1974,24 +2039,24 @@
       <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="54"/>
-      <c r="T13" s="54"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
+      <c r="AA13" s="55"/>
+      <c r="AB13" s="55"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="2"/>
@@ -2005,11 +2070,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AH2"/>
@@ -2025,6 +2085,11 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.39374999999999999" bottom="0.39374999999999999" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2037,17 +2102,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.08984375" style="38" customWidth="1"/>
     <col min="2" max="2" width="10.1796875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="81.1796875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="88.1796875" style="38" customWidth="1"/>
     <col min="4" max="4" width="16.7265625" style="38" customWidth="1"/>
     <col min="5" max="6" width="10.1796875" style="38" customWidth="1"/>
     <col min="7" max="7" width="18.7265625" style="38" customWidth="1"/>
@@ -3082,13 +3147,260 @@
         <v>44992</v>
       </c>
       <c r="F46" s="40">
-        <f>F45</f>
-        <v>45006</v>
+        <v>45013</v>
       </c>
       <c r="G46" s="41" t="str">
         <f>G45</f>
         <v>Terminer</v>
       </c>
+    </row>
+    <row r="47" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="39"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+    </row>
+    <row r="48" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="39">
+        <f>A46+1</f>
+        <v>37</v>
+      </c>
+      <c r="B48" s="40">
+        <v>45013</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="39"/>
+      <c r="E48" s="40">
+        <v>45020</v>
+      </c>
+      <c r="F48" s="39"/>
+      <c r="G48" s="60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="39">
+        <f>A48+1</f>
+        <v>38</v>
+      </c>
+      <c r="B49" s="40">
+        <f>B48</f>
+        <v>45013</v>
+      </c>
+      <c r="C49" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="39"/>
+      <c r="E49" s="40">
+        <f>E48</f>
+        <v>45020</v>
+      </c>
+      <c r="F49" s="39"/>
+      <c r="G49" s="60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="39">
+        <f t="shared" ref="A50:A54" si="7">A49+1</f>
+        <v>39</v>
+      </c>
+      <c r="B50" s="40">
+        <f t="shared" ref="B50:B54" si="8">B49</f>
+        <v>45013</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="39"/>
+      <c r="E50" s="40">
+        <f t="shared" ref="E50:E54" si="9">E49</f>
+        <v>45020</v>
+      </c>
+      <c r="F50" s="59"/>
+      <c r="G50" s="60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="39">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="B51" s="40">
+        <f t="shared" si="8"/>
+        <v>45013</v>
+      </c>
+      <c r="C51" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="39"/>
+      <c r="E51" s="40">
+        <f t="shared" si="9"/>
+        <v>45020</v>
+      </c>
+      <c r="F51" s="59"/>
+      <c r="G51" s="61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="39">
+        <f t="shared" si="7"/>
+        <v>41</v>
+      </c>
+      <c r="B52" s="40">
+        <f t="shared" si="8"/>
+        <v>45013</v>
+      </c>
+      <c r="C52" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D52" s="39"/>
+      <c r="E52" s="40">
+        <f t="shared" si="9"/>
+        <v>45020</v>
+      </c>
+      <c r="F52" s="59"/>
+      <c r="G52" s="60" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="39">
+        <f t="shared" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="B53" s="40">
+        <f t="shared" si="8"/>
+        <v>45013</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="39"/>
+      <c r="E53" s="40">
+        <f t="shared" si="9"/>
+        <v>45020</v>
+      </c>
+      <c r="F53" s="59"/>
+      <c r="G53" s="61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="39">
+        <f t="shared" si="7"/>
+        <v>43</v>
+      </c>
+      <c r="B54" s="40">
+        <f t="shared" si="8"/>
+        <v>45013</v>
+      </c>
+      <c r="C54" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="39"/>
+      <c r="E54" s="40">
+        <f t="shared" si="9"/>
+        <v>45020</v>
+      </c>
+      <c r="F54" s="59"/>
+      <c r="G54" s="61" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="39"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+    </row>
+    <row r="56" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="39"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+    </row>
+    <row r="57" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="58"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+    </row>
+    <row r="58" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
+    </row>
+    <row r="59" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="58"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="58"/>
+    </row>
+    <row r="60" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="58"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+    </row>
+    <row r="61" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="58"/>
+      <c r="B61" s="58"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="58"/>
+    </row>
+    <row r="62" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="58"/>
+      <c r="B62" s="58"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="58"/>
+    </row>
+    <row r="63" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="58"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="58"/>
+    </row>
+    <row r="64" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="58"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="58"/>
+    </row>
+    <row r="65" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="58"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3119,74 +3431,74 @@
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="55" t="s">
+      <c r="F3" s="56"/>
+      <c r="G3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="53" t="s">
+      <c r="H3" s="52"/>
+      <c r="I3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53" t="s">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="55" t="s">
+      <c r="L3" s="54"/>
+      <c r="M3" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55" t="s">
+      <c r="N3" s="52"/>
+      <c r="O3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55" t="s">
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="55"/>
-      <c r="S3" s="55" t="s">
+      <c r="R3" s="52"/>
+      <c r="S3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="53" t="s">
+      <c r="T3" s="52"/>
+      <c r="U3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="53"/>
-      <c r="W3" s="55" t="s">
+      <c r="V3" s="54"/>
+      <c r="W3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="53" t="s">
+      <c r="X3" s="52"/>
+      <c r="Y3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="53"/>
-      <c r="AA3" s="55" t="s">
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="55"/>
-      <c r="AC3" s="53" t="s">
+      <c r="AB3" s="52"/>
+      <c r="AC3" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="53"/>
-      <c r="AE3" s="53" t="s">
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53" t="s">
+      <c r="AF3" s="54"/>
+      <c r="AG3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="53" t="s">
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="AJ3" s="53"/>
+      <c r="AJ3" s="54"/>
     </row>
     <row r="4" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -3203,30 +3515,30 @@
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="54"/>
+      <c r="L4" s="55"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="54" t="s">
+      <c r="S4" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="54"/>
+      <c r="T4" s="55"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-      <c r="AA4" s="54" t="s">
+      <c r="AA4" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="54"/>
+      <c r="AB4" s="55"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -3251,24 +3563,24 @@
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
+      <c r="AA5" s="55"/>
+      <c r="AB5" s="55"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -3293,24 +3605,24 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
       <c r="M6" s="2"/>
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="54"/>
+      <c r="AA6" s="55"/>
+      <c r="AB6" s="55"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -3335,24 +3647,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
       <c r="M7" s="2"/>
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="54"/>
-      <c r="T7" s="54"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
       <c r="U7" s="2"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="54"/>
-      <c r="AB7" s="54"/>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="55"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -3377,24 +3689,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
       <c r="M8" s="9"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
       <c r="U8" s="2"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="54"/>
-      <c r="AB8" s="54"/>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="55"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -3419,24 +3731,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
       <c r="U9" s="13"/>
       <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-      <c r="AA9" s="54"/>
-      <c r="AB9" s="54"/>
+      <c r="AA9" s="55"/>
+      <c r="AB9" s="55"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="5"/>
       <c r="AE9" s="2"/>
@@ -3461,24 +3773,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="55"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="54"/>
-      <c r="T10" s="54"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
       <c r="U10" s="2"/>
       <c r="V10" s="5"/>
       <c r="W10" s="9"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="11"/>
-      <c r="AA10" s="54"/>
-      <c r="AB10" s="54"/>
+      <c r="AA10" s="55"/>
+      <c r="AB10" s="55"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="2"/>
@@ -3503,24 +3815,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="55"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="54"/>
-      <c r="AB11" s="54"/>
+      <c r="AA11" s="55"/>
+      <c r="AB11" s="55"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="11"/>
       <c r="AE11" s="2"/>
@@ -3543,24 +3855,24 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
       <c r="M12" s="13"/>
       <c r="N12" s="12"/>
       <c r="O12" s="13"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="54"/>
-      <c r="T12" s="54"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="55"/>
       <c r="U12" s="13"/>
       <c r="V12" s="10"/>
       <c r="W12" s="13"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="54"/>
-      <c r="AB12" s="54"/>
+      <c r="AA12" s="55"/>
+      <c r="AB12" s="55"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="2"/>
@@ -3583,24 +3895,24 @@
       <c r="H13" s="6"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="55"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="54"/>
-      <c r="T13" s="54"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
+      <c r="AA13" s="55"/>
+      <c r="AB13" s="55"/>
       <c r="AC13" s="9"/>
       <c r="AD13" s="11"/>
       <c r="AE13" s="2"/>
@@ -3623,24 +3935,24 @@
       <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
       <c r="U14" s="2"/>
       <c r="V14" s="5"/>
       <c r="W14" s="2"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-      <c r="AA14" s="54"/>
-      <c r="AB14" s="54"/>
+      <c r="AA14" s="55"/>
+      <c r="AB14" s="55"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="9"/>
@@ -3654,11 +3966,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="20">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AG3:AH3"/>
@@ -3674,6 +3981,11 @@
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.39374999999999999" bottom="0.39374999999999999" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
correction courbe_bezier_sam + ajoue fichier-resul
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samle\VSC-Rpertoire\MAP401\bitmap-vectoriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490718E6-77E4-4E6A-A50C-05C956EAAB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7BFD0D-F25D-42CC-B0C5-54126B03878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="119">
   <si>
     <t>s3</t>
   </si>
@@ -329,9 +329,6 @@
     <t>TACHE 6 Partie 1</t>
   </si>
   <si>
-    <t xml:space="preserve">En cours </t>
-  </si>
-  <si>
     <t xml:space="preserve">Compléter le module 2D </t>
   </si>
   <si>
@@ -361,13 +358,6 @@
   </si>
   <si>
     <t>Terminer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quand on aura le 
-temps on le fera </t>
-  </si>
-  <si>
-    <t>mettre en place une fonction pour créer les fichiers tests (Non obligatoire)</t>
   </si>
   <si>
     <r>
@@ -618,12 +608,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -634,8 +618,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -963,6 +953,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -975,7 +1004,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1022,11 +1051,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1053,17 +1078,35 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1081,22 +1124,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="En-tête" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1109,8 +1139,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFFF9900"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1512,7 +1542,7 @@
   <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1526,80 +1556,80 @@
   <sheetData>
     <row r="1" spans="1:36" ht="108.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52" t="s">
+      <c r="F2" s="56"/>
+      <c r="G2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="54" t="s">
+      <c r="H2" s="56"/>
+      <c r="I2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="52" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="54" t="s">
+      <c r="L2" s="56"/>
+      <c r="M2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="54"/>
-      <c r="O2" s="52" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52" t="s">
+      <c r="P2" s="56"/>
+      <c r="Q2" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52" t="s">
+      <c r="R2" s="57"/>
+      <c r="S2" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="52"/>
-      <c r="U2" s="54" t="s">
+      <c r="T2" s="56"/>
+      <c r="U2" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="52" t="s">
+      <c r="V2" s="58"/>
+      <c r="W2" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="54" t="s">
+      <c r="X2" s="56"/>
+      <c r="Y2" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="52" t="s">
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="54" t="s">
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54" t="s">
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54" t="s">
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54" t="s">
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="54"/>
+      <c r="AJ2" s="58"/>
     </row>
     <row r="3" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1616,30 +1646,30 @@
       <c r="H3" s="5"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="55"/>
+      <c r="L3" s="59"/>
       <c r="M3" s="2"/>
       <c r="N3" s="5"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="55" t="s">
+      <c r="P3" s="6"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="55"/>
+      <c r="T3" s="59"/>
       <c r="U3" s="2"/>
       <c r="V3" s="5"/>
       <c r="W3" s="2"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="55" t="s">
+      <c r="AA3" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="55"/>
+      <c r="AB3" s="59"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="2"/>
@@ -1664,24 +1694,24 @@
       <c r="H4" s="19"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -1706,24 +1736,24 @@
       <c r="H5" s="24"/>
       <c r="I5" s="27"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -1748,24 +1778,24 @@
       <c r="H6" s="21"/>
       <c r="I6" s="28"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
       <c r="M6" s="29"/>
       <c r="N6" s="19"/>
       <c r="O6" s="29"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="55"/>
-      <c r="AB6" s="55"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -1790,23 +1820,23 @@
       <c r="H7" s="5"/>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
       <c r="M7" s="23"/>
       <c r="N7" s="30"/>
       <c r="O7" s="19"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
       <c r="U7" s="29"/>
       <c r="V7" s="19"/>
       <c r="W7" s="29"/>
       <c r="X7" s="19"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="55"/>
-      <c r="AB7" s="55"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -1831,24 +1861,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="17"/>
       <c r="N8" s="21"/>
       <c r="O8" s="31"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="23"/>
       <c r="V8" s="62"/>
-      <c r="W8" s="57"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="55"/>
-      <c r="AB8" s="55"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="59"/>
+      <c r="AB8" s="59"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -1862,7 +1892,7 @@
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="32" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="2"/>
@@ -1873,24 +1903,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="17"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="63"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="44"/>
-      <c r="Z9" s="32"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="55"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="59"/>
+      <c r="AB9" s="59"/>
       <c r="AC9" s="29"/>
       <c r="AD9" s="19"/>
       <c r="AE9" s="29"/>
@@ -1904,7 +1934,7 @@
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2"/>
@@ -1915,28 +1945,28 @@
       <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
       <c r="U10" s="17"/>
       <c r="V10" s="20"/>
       <c r="W10" s="17"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="17"/>
       <c r="Z10" s="20"/>
-      <c r="AA10" s="55"/>
-      <c r="AB10" s="55"/>
-      <c r="AC10" s="47"/>
-      <c r="AD10" s="48"/>
-      <c r="AE10" s="49"/>
-      <c r="AF10" s="50"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="59"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="44"/>
+      <c r="AF10" s="45"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="5"/>
       <c r="AI10" s="2"/>
@@ -1946,7 +1976,7 @@
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="46" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2"/>
@@ -1957,28 +1987,28 @@
       <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="55"/>
-      <c r="AB11" s="55"/>
-      <c r="AC11" s="47"/>
-      <c r="AD11" s="48"/>
-      <c r="AE11" s="49"/>
-      <c r="AF11" s="50"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="59"/>
+      <c r="AC11" s="42"/>
+      <c r="AD11" s="43"/>
+      <c r="AE11" s="44"/>
+      <c r="AF11" s="45"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="5"/>
       <c r="AI11" s="2"/>
@@ -1999,24 +2029,24 @@
       <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
       <c r="M12" s="2"/>
       <c r="N12" s="5"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
       <c r="U12" s="2"/>
       <c r="V12" s="5"/>
       <c r="W12" s="2"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="5"/>
-      <c r="AA12" s="55"/>
-      <c r="AB12" s="55"/>
+      <c r="AA12" s="59"/>
+      <c r="AB12" s="59"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="20"/>
       <c r="AE12" s="17"/>
@@ -2039,24 +2069,24 @@
       <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="55"/>
-      <c r="AB13" s="55"/>
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="59"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="2"/>
@@ -2102,1305 +2132,1284 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" style="38" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="88.1796875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" style="38" customWidth="1"/>
-    <col min="5" max="6" width="10.1796875" style="38" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" style="38" customWidth="1"/>
-    <col min="8" max="16384" width="11.54296875" style="38"/>
+    <col min="1" max="1" width="5.08984375" style="36" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="88.1796875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" style="36" customWidth="1"/>
+    <col min="5" max="6" width="10.1796875" style="36" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" style="36" customWidth="1"/>
+    <col min="8" max="16384" width="11.54296875" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:7" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="55" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36" t="s">
+    <row r="2" spans="1:7" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+      <c r="A3" s="37">
         <v>1</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="38">
         <v>44950</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="40">
+      <c r="D3" s="37"/>
+      <c r="E3" s="38">
         <v>44950</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="38">
         <v>44950</v>
       </c>
-      <c r="G3" s="41" t="s">
-        <v>106</v>
+      <c r="G3" s="39" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
+      <c r="A4" s="37">
         <v>2</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="38">
         <f>B3</f>
         <v>44950</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40">
+      <c r="D4" s="37"/>
+      <c r="E4" s="38">
         <f>E3</f>
         <v>44950</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="38">
         <f>F3</f>
         <v>44950</v>
       </c>
-      <c r="G4" s="42" t="str">
+      <c r="G4" s="40" t="str">
         <f>G3</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="37" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="37">
         <v>3</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="38">
         <f>B4</f>
         <v>44950</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40">
+      <c r="D6" s="37"/>
+      <c r="E6" s="38">
         <f>E4</f>
         <v>44950</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="38">
         <f>F4</f>
         <v>44950</v>
       </c>
-      <c r="G6" s="42" t="str">
+      <c r="G6" s="40" t="str">
         <f>G4</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="37">
         <v>4</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="38">
         <f>B6</f>
         <v>44950</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40">
+      <c r="D7" s="37"/>
+      <c r="E7" s="38">
         <f>E6</f>
         <v>44950</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="38">
         <f t="shared" ref="F7:G9" si="0">F6</f>
         <v>44950</v>
       </c>
-      <c r="G7" s="42" t="str">
+      <c r="G7" s="40" t="str">
         <f t="shared" si="0"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+      <c r="A8" s="37">
         <v>5</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="38">
         <f>B7</f>
         <v>44950</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40">
+      <c r="D8" s="37"/>
+      <c r="E8" s="38">
         <f>E7</f>
         <v>44950</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="38">
         <f t="shared" si="0"/>
         <v>44950</v>
       </c>
-      <c r="G8" s="42" t="str">
+      <c r="G8" s="40" t="str">
         <f t="shared" si="0"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="37">
         <v>6</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="38">
         <f>B6</f>
         <v>44950</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40">
+      <c r="D9" s="37"/>
+      <c r="E9" s="38">
         <f>E8</f>
         <v>44950</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="38">
         <f t="shared" si="0"/>
         <v>44950</v>
       </c>
-      <c r="G9" s="42" t="str">
+      <c r="G9" s="40" t="str">
         <f>G8</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="37" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="37">
         <v>7</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="38">
         <v>44957</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="40">
+      <c r="D11" s="37"/>
+      <c r="E11" s="38">
         <v>44957</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="38">
         <f>E11</f>
         <v>44957</v>
       </c>
-      <c r="G11" s="42" t="str">
+      <c r="G11" s="40" t="str">
         <f>G9</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="37">
         <f>A11+1</f>
         <v>8</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="38">
         <f>B11</f>
         <v>44957</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40">
+      <c r="D12" s="37"/>
+      <c r="E12" s="38">
         <f>E11</f>
         <v>44957</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="38">
         <f t="shared" ref="F12:G20" si="1">F11</f>
         <v>44957</v>
       </c>
-      <c r="G12" s="42" t="str">
+      <c r="G12" s="40" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
+      <c r="A13" s="37">
         <f>A12+1</f>
         <v>9</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="38">
         <f>B12</f>
         <v>44957</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40">
+      <c r="D13" s="37"/>
+      <c r="E13" s="38">
         <f>E12</f>
         <v>44957</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="38">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G13" s="42" t="str">
+      <c r="G13" s="40" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="37">
         <f t="shared" ref="A14:A20" si="2">A13+1</f>
         <v>10</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="38">
         <f t="shared" ref="B14:B20" si="3">B13</f>
         <v>44957</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40">
+      <c r="D14" s="37"/>
+      <c r="E14" s="38">
         <f t="shared" ref="E14:E20" si="4">E13</f>
         <v>44957</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="38">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G14" s="42" t="str">
+      <c r="G14" s="40" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="37" t="s">
+      <c r="A15" s="37"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="A16" s="37">
         <f>A14+1</f>
         <v>11</v>
       </c>
-      <c r="B16" s="40">
+      <c r="B16" s="38">
         <f>B14</f>
         <v>44957</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40">
+      <c r="D16" s="37"/>
+      <c r="E16" s="38">
         <f>E14</f>
         <v>44957</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="38">
         <f>F14</f>
         <v>44957</v>
       </c>
-      <c r="G16" s="42" t="str">
+      <c r="G16" s="40" t="str">
         <f>G14</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39">
+      <c r="A17" s="37">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B17" s="40">
+      <c r="B17" s="38">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40">
+      <c r="D17" s="37"/>
+      <c r="E17" s="38">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="38">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G17" s="42" t="str">
+      <c r="G17" s="40" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="37">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="38">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40">
+      <c r="D18" s="37"/>
+      <c r="E18" s="38">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="38">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G18" s="42" t="str">
+      <c r="G18" s="40" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="37">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="38">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40">
+      <c r="D19" s="37"/>
+      <c r="E19" s="38">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="38">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G19" s="42" t="str">
+      <c r="G19" s="40" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39">
+      <c r="A20" s="37">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B20" s="40">
+      <c r="B20" s="38">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40">
+      <c r="D20" s="37"/>
+      <c r="E20" s="38">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F20" s="40">
+      <c r="F20" s="38">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G20" s="42" t="str">
+      <c r="G20" s="40" t="str">
         <f>G19</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="37" t="s">
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
     </row>
     <row r="22" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="37">
         <f>A20+1</f>
         <v>16</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="38">
         <v>44964</v>
       </c>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40">
+      <c r="D22" s="37"/>
+      <c r="E22" s="38">
         <f>B22</f>
         <v>44964</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="38">
         <f>E22</f>
         <v>44964</v>
       </c>
-      <c r="G22" s="42" t="str">
+      <c r="G22" s="40" t="str">
         <f>G20</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+      <c r="A23" s="37">
         <f>A22+1</f>
         <v>17</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="38">
         <f>B22</f>
         <v>44964</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40">
+      <c r="D23" s="37"/>
+      <c r="E23" s="38">
         <f>B23</f>
         <v>44964</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="38">
         <f>E23</f>
         <v>44964</v>
       </c>
-      <c r="G23" s="42" t="str">
+      <c r="G23" s="40" t="str">
         <f>G22</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+      <c r="A24" s="37">
         <f>A23+1</f>
         <v>18</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="38">
         <f>B23</f>
         <v>44964</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40">
+      <c r="D24" s="37"/>
+      <c r="E24" s="38">
         <f>B24</f>
         <v>44964</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="38">
         <f>E24</f>
         <v>44964</v>
       </c>
-      <c r="G24" s="42" t="str">
+      <c r="G24" s="40" t="str">
         <f>G22</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39">
+      <c r="A25" s="37">
         <f>A24+1</f>
         <v>19</v>
       </c>
-      <c r="B25" s="40">
+      <c r="B25" s="38">
         <f>B24</f>
         <v>44964</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40">
+      <c r="D25" s="37"/>
+      <c r="E25" s="38">
         <f>B25</f>
         <v>44964</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="38">
         <f>E25</f>
         <v>44964</v>
       </c>
-      <c r="G25" s="42" t="str">
+      <c r="G25" s="40" t="str">
         <f>G23</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="37" t="s">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
     </row>
     <row r="27" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39">
+      <c r="A27" s="37">
         <f>A25+1</f>
         <v>20</v>
       </c>
-      <c r="B27" s="40">
+      <c r="B27" s="38">
         <f>B25</f>
         <v>44964</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40">
+      <c r="D27" s="37"/>
+      <c r="E27" s="38">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="F27" s="40">
+      <c r="F27" s="38">
         <f t="shared" ref="F27:F32" si="5">E27</f>
         <v>44964</v>
       </c>
-      <c r="G27" s="42" t="str">
+      <c r="G27" s="40" t="str">
         <f>G25</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="39">
-        <f t="shared" ref="A28:A33" si="6">A27+1</f>
+      <c r="A28" s="37">
+        <f t="shared" ref="A28:A32" si="6">A27+1</f>
         <v>21</v>
       </c>
-      <c r="B28" s="40">
+      <c r="B28" s="38">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="40">
+      <c r="D28" s="37"/>
+      <c r="E28" s="38">
         <v>44978</v>
       </c>
-      <c r="F28" s="40">
+      <c r="F28" s="38">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G28" s="42" t="str">
+      <c r="G28" s="40" t="str">
         <f>G27</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="39">
+      <c r="A29" s="37">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="B29" s="40">
+      <c r="B29" s="38">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="40">
+      <c r="D29" s="37"/>
+      <c r="E29" s="38">
         <f>E28</f>
         <v>44978</v>
       </c>
-      <c r="F29" s="40">
+      <c r="F29" s="38">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G29" s="42" t="str">
+      <c r="G29" s="40" t="str">
         <f>G28</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="48.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+      <c r="A30" s="37">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="B30" s="40">
+      <c r="B30" s="38">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="40">
+      <c r="E30" s="38">
         <f>E29</f>
         <v>44978</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="38">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G30" s="42" t="str">
+      <c r="G30" s="40" t="str">
         <f>G29</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="37">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="B31" s="40">
+      <c r="B31" s="38">
         <f>B29</f>
         <v>44964</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="39"/>
-      <c r="E31" s="40">
+      <c r="D31" s="37"/>
+      <c r="E31" s="38">
         <f>E30</f>
         <v>44978</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="38">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G31" s="42" t="str">
+      <c r="G31" s="40" t="str">
         <f>G30</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="39">
+      <c r="A32" s="37">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="B32" s="40">
+      <c r="B32" s="38">
         <v>44985</v>
       </c>
-      <c r="C32" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="40">
+      <c r="C32" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="37"/>
+      <c r="E32" s="38">
         <f>B32</f>
         <v>44985</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="38">
         <f t="shared" si="5"/>
         <v>44985</v>
       </c>
-      <c r="G32" s="42" t="str">
+      <c r="G32" s="40" t="str">
         <f>G31</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="39">
-        <f t="shared" si="6"/>
-        <v>26</v>
-      </c>
-      <c r="B33" s="40">
-        <f>B32</f>
-        <v>44985</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="43" t="s">
-        <v>96</v>
-      </c>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
     </row>
     <row r="34" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-    </row>
-    <row r="35" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="39">
-        <f>A33+1</f>
-        <v>27</v>
-      </c>
-      <c r="B35" s="40">
+      <c r="A34" s="37" t="e">
+        <f>#REF!+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B34" s="38">
         <f>E28</f>
         <v>44978</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C34" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="40">
+      <c r="D34" s="37"/>
+      <c r="E34" s="38">
         <f>E31</f>
         <v>44978</v>
       </c>
-      <c r="F35" s="40">
+      <c r="F34" s="38">
+        <f>E34</f>
+        <v>44978</v>
+      </c>
+      <c r="G34" s="40" t="str">
+        <f>G30</f>
+        <v>Terminer</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="e">
+        <f>A34+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B35" s="38">
+        <f>B34</f>
+        <v>44978</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="37"/>
+      <c r="E35" s="38">
+        <f>E34</f>
+        <v>44978</v>
+      </c>
+      <c r="F35" s="38">
         <f>E35</f>
         <v>44978</v>
       </c>
-      <c r="G35" s="42" t="str">
-        <f>G30</f>
+      <c r="G35" s="39" t="str">
+        <f>G34</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39">
+      <c r="A36" s="37" t="e">
         <f>A35+1</f>
-        <v>28</v>
-      </c>
-      <c r="B36" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B36" s="38">
         <f>B35</f>
         <v>44978</v>
       </c>
-      <c r="C36" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="40">
+      <c r="C36" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="37"/>
+      <c r="E36" s="38">
         <f>E35</f>
         <v>44978</v>
       </c>
-      <c r="F36" s="40">
+      <c r="F36" s="38">
         <f>E36</f>
         <v>44978</v>
       </c>
-      <c r="G36" s="41" t="str">
+      <c r="G36" s="39" t="str">
         <f>G35</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39">
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+    </row>
+    <row r="38" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="37" t="e">
         <f>A36+1</f>
-        <v>29</v>
-      </c>
-      <c r="B37" s="40">
-        <f>B36</f>
-        <v>44978</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="40">
-        <f>E36</f>
-        <v>44978</v>
-      </c>
-      <c r="F37" s="40">
-        <f>E37</f>
-        <v>44978</v>
-      </c>
-      <c r="G37" s="41" t="str">
+        <v>#REF!</v>
+      </c>
+      <c r="B38" s="38">
+        <v>44985</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="37"/>
+      <c r="E38" s="38">
+        <f>B38</f>
+        <v>44985</v>
+      </c>
+      <c r="F38" s="38">
+        <f>E38</f>
+        <v>44985</v>
+      </c>
+      <c r="G38" s="39" t="str">
         <f>G36</f>
         <v>Terminer</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-    </row>
     <row r="39" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39">
-        <f>A37+1</f>
-        <v>30</v>
-      </c>
-      <c r="B39" s="40">
+      <c r="A39" s="37" t="e">
+        <f>A38+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B39" s="38">
+        <f>B38</f>
         <v>44985</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="40">
+      <c r="D39" s="37"/>
+      <c r="E39" s="38">
         <f>B39</f>
         <v>44985</v>
       </c>
-      <c r="F39" s="40">
+      <c r="F39" s="38">
         <f>E39</f>
         <v>44985</v>
       </c>
-      <c r="G39" s="41" t="str">
-        <f>G37</f>
+      <c r="G39" s="39" t="str">
+        <f>G38</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39">
+      <c r="A40" s="37" t="e">
         <f>A39+1</f>
-        <v>31</v>
-      </c>
-      <c r="B40" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B40" s="38">
         <f>B39</f>
         <v>44985</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="39"/>
-      <c r="E40" s="40">
+      <c r="D40" s="37"/>
+      <c r="E40" s="38">
         <f>B40</f>
         <v>44985</v>
       </c>
-      <c r="F40" s="40">
+      <c r="F40" s="38">
         <f>E40</f>
         <v>44985</v>
       </c>
-      <c r="G40" s="41" t="str">
+      <c r="G40" s="39" t="str">
         <f>G39</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39">
+      <c r="A41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+    </row>
+    <row r="42" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="e">
         <f>A40+1</f>
-        <v>32</v>
-      </c>
-      <c r="B41" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B42" s="38">
         <f>B40</f>
         <v>44985</v>
       </c>
-      <c r="C41" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="40">
-        <f>B41</f>
-        <v>44985</v>
-      </c>
-      <c r="F41" s="40">
-        <f>E41</f>
-        <v>44985</v>
-      </c>
-      <c r="G41" s="41" t="str">
+      <c r="C42" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="37"/>
+      <c r="E42" s="38">
+        <v>44992</v>
+      </c>
+      <c r="F42" s="38">
+        <v>45006</v>
+      </c>
+      <c r="G42" s="39" t="str">
         <f>G40</f>
         <v>Terminer</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="39"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-    </row>
     <row r="43" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39">
-        <f>A41+1</f>
-        <v>33</v>
-      </c>
-      <c r="B43" s="40">
-        <f>B41</f>
+      <c r="A43" s="37" t="e">
+        <f>A42+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B43" s="38">
+        <f>B42</f>
         <v>44985</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="40">
+      <c r="D43" s="37"/>
+      <c r="E43" s="38">
+        <f>E42</f>
         <v>44992</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="38">
+        <f>+F42</f>
         <v>45006</v>
       </c>
-      <c r="G43" s="41" t="str">
-        <f>G41</f>
+      <c r="G43" s="39" t="str">
+        <f>G42</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39">
+      <c r="A44" s="37" t="e">
         <f>A43+1</f>
-        <v>34</v>
-      </c>
-      <c r="B44" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B44" s="38">
         <f>B43</f>
         <v>44985</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="40">
+      <c r="D44" s="37"/>
+      <c r="E44" s="38">
         <f>E43</f>
         <v>44992</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="38">
         <f>+F43</f>
         <v>45006</v>
       </c>
-      <c r="G44" s="41" t="str">
-        <f>G43</f>
+      <c r="G44" s="39" t="str">
+        <f>G42</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39">
+      <c r="A45" s="37" t="e">
         <f>A44+1</f>
-        <v>35</v>
-      </c>
-      <c r="B45" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B45" s="38">
         <f>B44</f>
         <v>44985</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="39"/>
-      <c r="E45" s="40">
+      <c r="D45" s="37"/>
+      <c r="E45" s="38">
         <f>E44</f>
         <v>44992</v>
       </c>
-      <c r="F45" s="40">
-        <f>+F44</f>
-        <v>45006</v>
-      </c>
-      <c r="G45" s="41" t="str">
-        <f>G43</f>
+      <c r="F45" s="38">
+        <v>45013</v>
+      </c>
+      <c r="G45" s="39" t="str">
+        <f>G44</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39">
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+    </row>
+    <row r="47" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="e">
         <f>A45+1</f>
-        <v>36</v>
-      </c>
-      <c r="B46" s="40">
-        <f>B45</f>
-        <v>44985</v>
-      </c>
-      <c r="C46" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="40">
-        <f>E45</f>
-        <v>44992</v>
-      </c>
-      <c r="F46" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B47" s="38">
         <v>45013</v>
       </c>
-      <c r="G46" s="41" t="str">
-        <f>G45</f>
-        <v>Terminer</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="37" t="s">
+      <c r="C47" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="37"/>
+      <c r="E47" s="38">
+        <v>45020</v>
+      </c>
+      <c r="F47" s="37"/>
+      <c r="G47" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="e">
+        <f>A47+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B48" s="38">
+        <f>B47</f>
+        <v>45013</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38">
+        <f>E47</f>
+        <v>45020</v>
+      </c>
+      <c r="F48" s="37"/>
+      <c r="G48" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="37" t="e">
+        <f t="shared" ref="A49:A53" si="7">A48+1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B49" s="38">
+        <f t="shared" ref="B49:B53" si="8">B48</f>
+        <v>45013</v>
+      </c>
+      <c r="C49" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-    </row>
-    <row r="48" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="39">
-        <f>A46+1</f>
-        <v>37</v>
-      </c>
-      <c r="B48" s="40">
-        <v>45013</v>
-      </c>
-      <c r="C48" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="40">
+      <c r="D49" s="37"/>
+      <c r="E49" s="38">
+        <f t="shared" ref="E49:E53" si="9">E48</f>
         <v>45020</v>
       </c>
-      <c r="F48" s="39"/>
-      <c r="G48" s="60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="39">
-        <f>A48+1</f>
-        <v>38</v>
-      </c>
-      <c r="B49" s="40">
-        <f>B48</f>
-        <v>45013</v>
-      </c>
-      <c r="C49" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="39"/>
-      <c r="E49" s="40">
-        <f>E48</f>
-        <v>45020</v>
-      </c>
-      <c r="F49" s="39"/>
-      <c r="G49" s="60" t="s">
-        <v>118</v>
+      <c r="F49" s="48"/>
+      <c r="G49" s="49" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39">
-        <f t="shared" ref="A50:A54" si="7">A49+1</f>
-        <v>39</v>
-      </c>
-      <c r="B50" s="40">
-        <f t="shared" ref="B50:B54" si="8">B49</f>
-        <v>45013</v>
-      </c>
-      <c r="C50" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" s="39"/>
-      <c r="E50" s="40">
-        <f t="shared" ref="E50:E54" si="9">E49</f>
-        <v>45020</v>
-      </c>
-      <c r="F50" s="59"/>
-      <c r="G50" s="60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="39">
+      <c r="A50" s="37" t="e">
         <f t="shared" si="7"/>
-        <v>40</v>
-      </c>
-      <c r="B51" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B50" s="38">
         <f t="shared" si="8"/>
         <v>45013</v>
       </c>
-      <c r="C51" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="39"/>
-      <c r="E51" s="40">
+      <c r="C50" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="37"/>
+      <c r="E50" s="38">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F51" s="59"/>
-      <c r="G51" s="61" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="39">
+      <c r="F50" s="48"/>
+      <c r="G50" s="50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="e">
         <f t="shared" si="7"/>
-        <v>41</v>
-      </c>
-      <c r="B52" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B51" s="38">
         <f t="shared" si="8"/>
         <v>45013</v>
       </c>
-      <c r="C52" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="39"/>
-      <c r="E52" s="40">
+      <c r="C51" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="37"/>
+      <c r="E51" s="38">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F52" s="59"/>
-      <c r="G52" s="60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39">
+      <c r="F51" s="48"/>
+      <c r="G51" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="e">
         <f t="shared" si="7"/>
-        <v>42</v>
-      </c>
-      <c r="B53" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B52" s="38">
         <f t="shared" si="8"/>
         <v>45013</v>
       </c>
-      <c r="C53" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="39"/>
-      <c r="E53" s="40">
+      <c r="C52" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="37"/>
+      <c r="E52" s="38">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F53" s="59"/>
-      <c r="G53" s="61" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="39">
+      <c r="F52" s="48"/>
+      <c r="G52" s="50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="e">
         <f t="shared" si="7"/>
-        <v>43</v>
-      </c>
-      <c r="B54" s="40">
+        <v>#REF!</v>
+      </c>
+      <c r="B53" s="38">
         <f t="shared" si="8"/>
         <v>45013</v>
       </c>
-      <c r="C54" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D54" s="39"/>
-      <c r="E54" s="40">
+      <c r="C53" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="37"/>
+      <c r="E53" s="38">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F54" s="59"/>
-      <c r="G54" s="61" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="59"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+    </row>
+    <row r="55" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="59"/>
+      <c r="A56" s="47"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
     </row>
     <row r="57" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="58"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
     </row>
     <row r="58" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="58"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
     </row>
     <row r="59" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="58"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
+      <c r="A59" s="47"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
     </row>
     <row r="60" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="58"/>
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
     </row>
     <row r="61" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
-      <c r="B61" s="58"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
+      <c r="A61" s="47"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
     </row>
     <row r="62" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="58"/>
-      <c r="B62" s="58"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="58"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
     </row>
     <row r="63" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="58"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
+      <c r="A63" s="47"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
     </row>
     <row r="64" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="58"/>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
-    </row>
-    <row r="65" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="58"/>
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
+      <c r="A64" s="47"/>
+      <c r="B64" s="47"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3417,7 +3426,7 @@
   </sheetPr>
   <dimension ref="A3:AJ65536"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="AL8" sqref="AL8"/>
     </sheetView>
   </sheetViews>
@@ -3431,74 +3440,74 @@
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="52" t="s">
+      <c r="F3" s="60"/>
+      <c r="G3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="54" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54" t="s">
+      <c r="J3" s="58"/>
+      <c r="K3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="54"/>
-      <c r="M3" s="52" t="s">
+      <c r="L3" s="58"/>
+      <c r="M3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52" t="s">
+      <c r="N3" s="56"/>
+      <c r="O3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52" t="s">
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52" t="s">
+      <c r="R3" s="56"/>
+      <c r="S3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="52"/>
-      <c r="U3" s="54" t="s">
+      <c r="T3" s="56"/>
+      <c r="U3" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="54"/>
-      <c r="W3" s="52" t="s">
+      <c r="V3" s="58"/>
+      <c r="W3" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="54" t="s">
+      <c r="X3" s="56"/>
+      <c r="Y3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="52" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="54" t="s">
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54" t="s">
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54" t="s">
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AJ3" s="54"/>
+      <c r="AJ3" s="58"/>
     </row>
     <row r="4" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -3515,30 +3524,30 @@
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="55" t="s">
+      <c r="K4" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="55"/>
+      <c r="L4" s="59"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="55" t="s">
+      <c r="S4" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="55"/>
+      <c r="T4" s="59"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-      <c r="AA4" s="55" t="s">
+      <c r="AA4" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="55"/>
+      <c r="AB4" s="59"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -3563,24 +3572,24 @@
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-      <c r="AA5" s="55"/>
-      <c r="AB5" s="55"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -3605,24 +3614,24 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
       <c r="M6" s="2"/>
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="55"/>
-      <c r="AB6" s="55"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -3647,24 +3656,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
       <c r="M7" s="2"/>
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="55"/>
-      <c r="T7" s="55"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
       <c r="U7" s="2"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="55"/>
-      <c r="AB7" s="55"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -3689,24 +3698,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="9"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="2"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="55"/>
-      <c r="AB8" s="55"/>
+      <c r="AA8" s="59"/>
+      <c r="AB8" s="59"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -3731,24 +3740,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="55"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
       <c r="U9" s="13"/>
       <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-      <c r="AA9" s="55"/>
-      <c r="AB9" s="55"/>
+      <c r="AA9" s="59"/>
+      <c r="AB9" s="59"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="5"/>
       <c r="AE9" s="2"/>
@@ -3773,24 +3782,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
       <c r="U10" s="2"/>
       <c r="V10" s="5"/>
       <c r="W10" s="9"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="11"/>
-      <c r="AA10" s="55"/>
-      <c r="AB10" s="55"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="59"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="2"/>
@@ -3815,24 +3824,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="55"/>
-      <c r="T11" s="55"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="55"/>
-      <c r="AB11" s="55"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="59"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="11"/>
       <c r="AE11" s="2"/>
@@ -3855,24 +3864,24 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
       <c r="M12" s="13"/>
       <c r="N12" s="12"/>
       <c r="O12" s="13"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
       <c r="U12" s="13"/>
       <c r="V12" s="10"/>
       <c r="W12" s="13"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="55"/>
-      <c r="AB12" s="55"/>
+      <c r="AA12" s="59"/>
+      <c r="AB12" s="59"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="2"/>
@@ -3895,24 +3904,24 @@
       <c r="H13" s="6"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-      <c r="AA13" s="55"/>
-      <c r="AB13" s="55"/>
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="59"/>
       <c r="AC13" s="9"/>
       <c r="AD13" s="11"/>
       <c r="AE13" s="2"/>
@@ -3935,24 +3944,24 @@
       <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
       <c r="U14" s="2"/>
       <c r="V14" s="5"/>
       <c r="W14" s="2"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-      <c r="AA14" s="55"/>
-      <c r="AB14" s="55"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="59"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="9"/>

</xml_diff>

<commit_message>
ajoue SP et modif bash
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samle\VSC-Rpertoire\MAP401\bitmap-vectoriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC2571B-A49A-4E48-AB0E-0D87432B59A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528EF58-FB3E-4C28-8A04-134D3419EF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiagrammeGanttReel" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="127">
   <si>
     <t>s3</t>
   </si>
@@ -504,16 +504,17 @@
 Test de performane et robustesse</t>
   </si>
   <si>
-    <t xml:space="preserve">Non Commencer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commenccer </t>
-  </si>
-  <si>
     <t>mettre les temps pour chaque image dans un pfd (ou leur erreurs)</t>
   </si>
   <si>
-    <t>terminer</t>
+    <t xml:space="preserve">Manque bezier 3 
+car ptobleme </t>
+  </si>
+  <si>
+    <t>Commencer</t>
+  </si>
+  <si>
+    <t>Presque Fini</t>
   </si>
 </sst>
 </file>
@@ -599,7 +600,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,18 +639,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -932,32 +927,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="hair">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1029,6 +998,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1041,7 +1050,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1116,8 +1125,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1128,33 +1135,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1163,17 +1172,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="En-tête" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1186,8 +1198,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FF00FF00"/>
-      <color rgb="FFFF9900"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1588,8 +1600,8 @@
   </sheetPr>
   <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1609,74 +1621,74 @@
     <row r="2" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62" t="s">
+      <c r="F2" s="60"/>
+      <c r="G2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="62"/>
-      <c r="I2" s="64" t="s">
+      <c r="H2" s="60"/>
+      <c r="I2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="64"/>
-      <c r="K2" s="62" t="s">
+      <c r="J2" s="58"/>
+      <c r="K2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="64" t="s">
+      <c r="L2" s="60"/>
+      <c r="M2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="64"/>
-      <c r="O2" s="62" t="s">
+      <c r="N2" s="58"/>
+      <c r="O2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="63" t="s">
+      <c r="P2" s="60"/>
+      <c r="Q2" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="63"/>
-      <c r="S2" s="62" t="s">
+      <c r="R2" s="61"/>
+      <c r="S2" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="U2" s="64" t="s">
+      <c r="T2" s="60"/>
+      <c r="U2" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="62" t="s">
+      <c r="V2" s="58"/>
+      <c r="W2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="64" t="s">
+      <c r="X2" s="60"/>
+      <c r="Y2" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="62" t="s">
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="64" t="s">
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64" t="s">
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="64" t="s">
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" s="64"/>
-      <c r="AI2" s="64" t="s">
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="64"/>
+      <c r="AJ2" s="58"/>
     </row>
     <row r="3" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1693,30 +1705,30 @@
       <c r="H3" s="5"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="65"/>
+      <c r="L3" s="59"/>
       <c r="M3" s="2"/>
       <c r="N3" s="5"/>
       <c r="O3" s="2"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="65" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="65"/>
+      <c r="T3" s="59"/>
       <c r="U3" s="2"/>
       <c r="V3" s="5"/>
       <c r="W3" s="2"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="65" t="s">
+      <c r="AA3" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="65"/>
+      <c r="AB3" s="59"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="2"/>
@@ -1741,24 +1753,24 @@
       <c r="H4" s="19"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="6"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="65"/>
-      <c r="AB4" s="65"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -1783,24 +1795,24 @@
       <c r="H5" s="24"/>
       <c r="I5" s="27"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -1825,24 +1837,24 @@
       <c r="H6" s="21"/>
       <c r="I6" s="28"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
       <c r="M6" s="29"/>
       <c r="N6" s="19"/>
       <c r="O6" s="29"/>
       <c r="P6" s="6"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="65"/>
-      <c r="AB6" s="65"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -1867,23 +1879,23 @@
       <c r="H7" s="5"/>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
       <c r="M7" s="23"/>
       <c r="N7" s="30"/>
       <c r="O7" s="19"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="65"/>
+      <c r="Q7" s="53"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
       <c r="U7" s="29"/>
       <c r="V7" s="19"/>
       <c r="W7" s="29"/>
       <c r="X7" s="19"/>
       <c r="Y7" s="29"/>
       <c r="Z7" s="19"/>
-      <c r="AA7" s="65"/>
-      <c r="AB7" s="65"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -1908,30 +1920,30 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="17"/>
       <c r="N8" s="21"/>
       <c r="O8" s="23"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="23"/>
-      <c r="V8" s="55"/>
-      <c r="W8" s="55"/>
-      <c r="X8" s="55"/>
-      <c r="Y8" s="55"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="52"/>
       <c r="Z8" s="24"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
+      <c r="AA8" s="59"/>
+      <c r="AB8" s="59"/>
       <c r="AC8" s="29"/>
       <c r="AD8" s="19"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="5"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="19"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="5"/>
     </row>
@@ -1950,31 +1962,31 @@
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="49"/>
-      <c r="V9" s="50"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="54"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="57"/>
-      <c r="AE9" s="22"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="5"/>
-      <c r="AI9" s="2"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+      <c r="X9" s="47"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="51"/>
+      <c r="AA9" s="59"/>
+      <c r="AB9" s="59"/>
+      <c r="AC9" s="64"/>
+      <c r="AD9" s="66"/>
+      <c r="AE9" s="66"/>
+      <c r="AF9" s="65"/>
+      <c r="AG9" s="41"/>
+      <c r="AH9" s="42"/>
+      <c r="AI9" s="6"/>
       <c r="AJ9" s="5"/>
     </row>
     <row r="10" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1992,38 +2004,38 @@
       <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
+      <c r="Q10" s="53"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
       <c r="U10" s="17"/>
       <c r="V10" s="20"/>
       <c r="W10" s="17"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="17"/>
       <c r="Z10" s="20"/>
-      <c r="AA10" s="65"/>
-      <c r="AB10" s="65"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="59"/>
       <c r="AC10" s="31"/>
-      <c r="AD10" s="57"/>
-      <c r="AE10" s="58"/>
-      <c r="AF10" s="44"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="2"/>
+      <c r="AD10" s="63"/>
+      <c r="AE10" s="63"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="71"/>
+      <c r="AH10" s="72"/>
+      <c r="AI10" s="6"/>
       <c r="AJ10" s="5"/>
     </row>
     <row r="11" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="68" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2"/>
@@ -2034,30 +2046,30 @@
       <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="42"/>
-      <c r="AE11" s="43"/>
-      <c r="AF11" s="44"/>
-      <c r="AG11" s="22"/>
-      <c r="AH11" s="19"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="59"/>
+      <c r="AC11" s="67"/>
+      <c r="AD11" s="67"/>
+      <c r="AE11" s="67"/>
+      <c r="AF11" s="67"/>
+      <c r="AG11" s="69"/>
+      <c r="AH11" s="70"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="5"/>
     </row>
@@ -2065,7 +2077,7 @@
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="43" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="2"/>
@@ -2076,36 +2088,36 @@
       <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
       <c r="M12" s="2"/>
       <c r="N12" s="5"/>
       <c r="O12" s="2"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
       <c r="U12" s="2"/>
       <c r="V12" s="5"/>
       <c r="W12" s="2"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="5"/>
-      <c r="AA12" s="65"/>
-      <c r="AB12" s="65"/>
+      <c r="AA12" s="59"/>
+      <c r="AB12" s="59"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="20"/>
       <c r="AE12" s="17"/>
       <c r="AF12" s="21"/>
       <c r="AG12" s="41"/>
-      <c r="AH12" s="44"/>
+      <c r="AH12" s="42"/>
       <c r="AI12" s="22"/>
       <c r="AJ12" s="19"/>
     </row>
     <row r="13" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="43" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="2"/>
@@ -2116,24 +2128,24 @@
       <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="65"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="65"/>
-      <c r="AB13" s="65"/>
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="59"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="2"/>
@@ -2141,12 +2153,17 @@
       <c r="AG13" s="17"/>
       <c r="AH13" s="21"/>
       <c r="AI13" s="41"/>
-      <c r="AJ13" s="44"/>
+      <c r="AJ13" s="42"/>
     </row>
     <row r="14" spans="1:36" ht="13" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AH2"/>
@@ -2162,11 +2179,6 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.39374999999999999" bottom="0.39374999999999999" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2181,8 +2193,8 @@
   </sheetPr>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView topLeftCell="A58" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2197,38 +2209,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="52" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
@@ -3237,7 +3249,10 @@
       <c r="E47" s="38">
         <v>45020</v>
       </c>
-      <c r="F47" s="37"/>
+      <c r="F47" s="38">
+        <f>F48</f>
+        <v>45034</v>
+      </c>
       <c r="G47" s="39" t="s">
         <v>105</v>
       </c>
@@ -3284,8 +3299,8 @@
         <v>45020</v>
       </c>
       <c r="F49" s="37"/>
-      <c r="G49" s="39" t="s">
-        <v>126</v>
+      <c r="G49" s="45" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -3355,21 +3370,24 @@
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F52" s="37"/>
+      <c r="F52" s="38">
+        <f>F51</f>
+        <v>45034</v>
+      </c>
       <c r="G52" s="39" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="59"/>
-      <c r="B53" s="59"/>
-      <c r="C53" s="60" t="s">
+      <c r="A53" s="55"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="67"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
     </row>
     <row r="54" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="37">
@@ -3387,8 +3405,8 @@
         <v>45048</v>
       </c>
       <c r="F54" s="37"/>
-      <c r="G54" s="39" t="s">
-        <v>105</v>
+      <c r="G54" s="45" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="71.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3418,9 +3436,11 @@
       <c r="E56" s="38">
         <v>45048</v>
       </c>
-      <c r="F56" s="37"/>
-      <c r="G56" s="47" t="s">
-        <v>124</v>
+      <c r="F56" s="38">
+        <v>45041</v>
+      </c>
+      <c r="G56" s="39" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -3439,9 +3459,12 @@
       <c r="E57" s="38">
         <v>45048</v>
       </c>
-      <c r="F57" s="37"/>
-      <c r="G57" s="47" t="s">
-        <v>124</v>
+      <c r="F57" s="38">
+        <f>F56</f>
+        <v>45041</v>
+      </c>
+      <c r="G57" s="39" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -3454,15 +3477,18 @@
         <v>45034</v>
       </c>
       <c r="C58" s="37" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D58" s="37"/>
       <c r="E58" s="38">
         <v>45048</v>
       </c>
-      <c r="F58" s="37"/>
-      <c r="G58" s="48" t="s">
-        <v>123</v>
+      <c r="F58" s="38">
+        <f>F57</f>
+        <v>45041</v>
+      </c>
+      <c r="G58" s="39" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3488,13 +3514,15 @@
       <c r="C60" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="37"/>
+      <c r="D60" s="33" t="s">
+        <v>124</v>
+      </c>
       <c r="E60" s="38">
         <v>45048</v>
       </c>
       <c r="F60" s="37"/>
-      <c r="G60" s="48" t="s">
-        <v>123</v>
+      <c r="G60" s="45" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -3514,8 +3542,9 @@
         <v>45048</v>
       </c>
       <c r="F61" s="37"/>
-      <c r="G61" s="48" t="s">
-        <v>123</v>
+      <c r="G61" s="45" t="str">
+        <f>G60</f>
+        <v>Commencer</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
@@ -3535,16 +3564,17 @@
         <v>45048</v>
       </c>
       <c r="F62" s="37"/>
-      <c r="G62" s="48" t="s">
-        <v>123</v>
+      <c r="G62" s="45" t="str">
+        <f>G61</f>
+        <v>Commencer</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="46"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
+      <c r="A63" s="44"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3575,74 +3605,74 @@
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66" t="s">
+      <c r="D3" s="62"/>
+      <c r="E3" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="62" t="s">
+      <c r="F3" s="62"/>
+      <c r="G3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="64" t="s">
+      <c r="H3" s="60"/>
+      <c r="I3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64" t="s">
+      <c r="J3" s="58"/>
+      <c r="K3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="62" t="s">
+      <c r="L3" s="58"/>
+      <c r="M3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62" t="s">
+      <c r="N3" s="60"/>
+      <c r="O3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62" t="s">
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62" t="s">
+      <c r="R3" s="60"/>
+      <c r="S3" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="62"/>
-      <c r="U3" s="64" t="s">
+      <c r="T3" s="60"/>
+      <c r="U3" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="64"/>
-      <c r="W3" s="62" t="s">
+      <c r="V3" s="58"/>
+      <c r="W3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="64" t="s">
+      <c r="X3" s="60"/>
+      <c r="Y3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="62" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="62"/>
-      <c r="AC3" s="64" t="s">
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64" t="s">
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64" t="s">
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64" t="s">
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="AJ3" s="64"/>
+      <c r="AJ3" s="58"/>
     </row>
     <row r="4" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -3659,30 +3689,30 @@
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="65"/>
+      <c r="L4" s="59"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="65" t="s">
+      <c r="S4" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="65"/>
+      <c r="T4" s="59"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-      <c r="AA4" s="65" t="s">
+      <c r="AA4" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="65"/>
+      <c r="AB4" s="59"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -3707,24 +3737,24 @@
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
+      <c r="AA5" s="59"/>
+      <c r="AB5" s="59"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -3749,24 +3779,24 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
       <c r="M6" s="2"/>
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="65"/>
-      <c r="AB6" s="65"/>
+      <c r="AA6" s="59"/>
+      <c r="AB6" s="59"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -3791,24 +3821,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
       <c r="M7" s="2"/>
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="65"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
       <c r="U7" s="2"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="65"/>
-      <c r="AB7" s="65"/>
+      <c r="AA7" s="59"/>
+      <c r="AB7" s="59"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -3833,24 +3863,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
       <c r="M8" s="9"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="65"/>
-      <c r="T8" s="65"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
       <c r="U8" s="2"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="65"/>
-      <c r="AB8" s="65"/>
+      <c r="AA8" s="59"/>
+      <c r="AB8" s="59"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -3875,24 +3905,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
+      <c r="S9" s="59"/>
+      <c r="T9" s="59"/>
       <c r="U9" s="13"/>
       <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="65"/>
+      <c r="AA9" s="59"/>
+      <c r="AB9" s="59"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="5"/>
       <c r="AE9" s="2"/>
@@ -3917,24 +3947,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
       <c r="U10" s="2"/>
       <c r="V10" s="5"/>
       <c r="W10" s="9"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="11"/>
-      <c r="AA10" s="65"/>
-      <c r="AB10" s="65"/>
+      <c r="AA10" s="59"/>
+      <c r="AB10" s="59"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="2"/>
@@ -3959,24 +3989,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="65"/>
-      <c r="AB11" s="65"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="59"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="11"/>
       <c r="AE11" s="2"/>
@@ -3999,24 +4029,24 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
       <c r="M12" s="13"/>
       <c r="N12" s="12"/>
       <c r="O12" s="13"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
       <c r="U12" s="13"/>
       <c r="V12" s="10"/>
       <c r="W12" s="13"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="65"/>
-      <c r="AB12" s="65"/>
+      <c r="AA12" s="59"/>
+      <c r="AB12" s="59"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="2"/>
@@ -4039,24 +4069,24 @@
       <c r="H13" s="6"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="65"/>
+      <c r="S13" s="59"/>
+      <c r="T13" s="59"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-      <c r="AA13" s="65"/>
-      <c r="AB13" s="65"/>
+      <c r="AA13" s="59"/>
+      <c r="AB13" s="59"/>
       <c r="AC13" s="9"/>
       <c r="AD13" s="11"/>
       <c r="AE13" s="2"/>
@@ -4079,24 +4109,24 @@
       <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="65"/>
-      <c r="T14" s="65"/>
+      <c r="S14" s="59"/>
+      <c r="T14" s="59"/>
       <c r="U14" s="2"/>
       <c r="V14" s="5"/>
       <c r="W14" s="2"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-      <c r="AA14" s="65"/>
-      <c r="AB14" s="65"/>
+      <c r="AA14" s="59"/>
+      <c r="AB14" s="59"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="9"/>
@@ -4110,6 +4140,11 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="20">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AG3:AH3"/>
@@ -4125,11 +4160,6 @@
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.39374999999999999" bottom="0.39374999999999999" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
version finale de l'excel
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samle\VSC-Rpertoire\MAP401\bitmap-vectoriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528EF58-FB3E-4C28-8A04-134D3419EF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E8DF64-C11A-4E98-9C44-6187FC0C7530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="778" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiagrammeGanttReel" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="126">
   <si>
     <t>s3</t>
   </si>
@@ -511,10 +511,7 @@
 car ptobleme </t>
   </si>
   <si>
-    <t>Commencer</t>
-  </si>
-  <si>
-    <t>Presque Fini</t>
+    <t xml:space="preserve">Terminer </t>
   </si>
 </sst>
 </file>
@@ -600,7 +597,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,18 +619,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,7 +1035,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1096,10 +1081,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1124,19 +1105,9 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1146,10 +1117,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1159,12 +1128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1172,20 +1136,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="En-tête" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1198,8 +1162,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FFFF9900"/>
-      <color rgb="FF00FF00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1600,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:AJ14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="67" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView zoomScale="58" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1621,74 +1585,74 @@
     <row r="2" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="58" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="60" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="58" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="58"/>
-      <c r="O2" s="60" t="s">
+      <c r="N2" s="51"/>
+      <c r="O2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="61" t="s">
+      <c r="P2" s="49"/>
+      <c r="Q2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="61"/>
-      <c r="S2" s="60" t="s">
+      <c r="R2" s="50"/>
+      <c r="S2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="60"/>
-      <c r="U2" s="58" t="s">
+      <c r="T2" s="49"/>
+      <c r="U2" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="58"/>
-      <c r="W2" s="60" t="s">
+      <c r="V2" s="51"/>
+      <c r="W2" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="58" t="s">
+      <c r="X2" s="49"/>
+      <c r="Y2" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="60" t="s">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="58" t="s">
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="58" t="s">
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AF2" s="58"/>
-      <c r="AG2" s="58" t="s">
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AH2" s="58"/>
-      <c r="AI2" s="58" t="s">
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AJ2" s="58"/>
+      <c r="AJ2" s="51"/>
     </row>
     <row r="3" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1705,30 +1669,30 @@
       <c r="H3" s="5"/>
       <c r="I3" s="2"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="59" t="s">
+      <c r="K3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="59"/>
+      <c r="L3" s="52"/>
       <c r="M3" s="2"/>
       <c r="N3" s="5"/>
       <c r="O3" s="2"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="53"/>
-      <c r="S3" s="59" t="s">
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="59"/>
+      <c r="T3" s="52"/>
       <c r="U3" s="2"/>
       <c r="V3" s="5"/>
       <c r="W3" s="2"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="59" t="s">
+      <c r="AA3" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AB3" s="59"/>
+      <c r="AB3" s="52"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="2"/>
@@ -1753,24 +1717,24 @@
       <c r="H4" s="19"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="6"/>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="52"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -1795,24 +1759,24 @@
       <c r="H5" s="24"/>
       <c r="I5" s="27"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="59"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="52"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -1837,24 +1801,24 @@
       <c r="H6" s="21"/>
       <c r="I6" s="28"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="29"/>
       <c r="N6" s="19"/>
       <c r="O6" s="29"/>
       <c r="P6" s="6"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="52"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -1879,23 +1843,23 @@
       <c r="H7" s="5"/>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
       <c r="M7" s="23"/>
       <c r="N7" s="30"/>
       <c r="O7" s="19"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
       <c r="U7" s="29"/>
       <c r="V7" s="19"/>
       <c r="W7" s="29"/>
       <c r="X7" s="19"/>
       <c r="Y7" s="29"/>
       <c r="Z7" s="19"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="59"/>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="52"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -1920,24 +1884,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="17"/>
       <c r="N8" s="21"/>
       <c r="O8" s="23"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="53"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="59"/>
-      <c r="T8" s="59"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
       <c r="U8" s="23"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="52"/>
-      <c r="Y8" s="52"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="43"/>
+      <c r="Y8" s="43"/>
       <c r="Z8" s="24"/>
-      <c r="AA8" s="59"/>
-      <c r="AB8" s="59"/>
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="52"/>
       <c r="AC8" s="29"/>
       <c r="AD8" s="19"/>
       <c r="AE8" s="29"/>
@@ -1951,7 +1915,7 @@
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="26" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="2"/>
@@ -1962,30 +1926,30 @@
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="17"/>
       <c r="P9" s="21"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="59"/>
-      <c r="T9" s="59"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="51"/>
-      <c r="AA9" s="59"/>
-      <c r="AB9" s="59"/>
-      <c r="AC9" s="64"/>
-      <c r="AD9" s="66"/>
-      <c r="AE9" s="66"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="41"/>
-      <c r="AH9" s="42"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="54"/>
+      <c r="V9" s="55"/>
+      <c r="W9" s="55"/>
+      <c r="X9" s="55"/>
+      <c r="Y9" s="55"/>
+      <c r="Z9" s="56"/>
+      <c r="AA9" s="52"/>
+      <c r="AB9" s="52"/>
+      <c r="AC9" s="57"/>
+      <c r="AD9" s="58"/>
+      <c r="AE9" s="58"/>
+      <c r="AF9" s="58"/>
+      <c r="AG9" s="58"/>
+      <c r="AH9" s="59"/>
       <c r="AI9" s="6"/>
       <c r="AJ9" s="5"/>
     </row>
@@ -1993,7 +1957,7 @@
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="2"/>
@@ -2004,30 +1968,30 @@
       <c r="H10" s="5"/>
       <c r="I10" s="2"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="6"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="52"/>
+      <c r="T10" s="52"/>
       <c r="U10" s="17"/>
       <c r="V10" s="20"/>
       <c r="W10" s="17"/>
       <c r="X10" s="20"/>
       <c r="Y10" s="17"/>
       <c r="Z10" s="20"/>
-      <c r="AA10" s="59"/>
-      <c r="AB10" s="59"/>
-      <c r="AC10" s="31"/>
-      <c r="AD10" s="63"/>
-      <c r="AE10" s="63"/>
-      <c r="AF10" s="54"/>
-      <c r="AG10" s="71"/>
-      <c r="AH10" s="72"/>
+      <c r="AA10" s="52"/>
+      <c r="AB10" s="52"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="43"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="24"/>
       <c r="AI10" s="6"/>
       <c r="AJ10" s="5"/>
     </row>
@@ -2035,7 +1999,7 @@
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2"/>
@@ -2046,30 +2010,25 @@
       <c r="H11" s="5"/>
       <c r="I11" s="2"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="52"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="59"/>
-      <c r="AB11" s="59"/>
-      <c r="AC11" s="67"/>
-      <c r="AD11" s="67"/>
-      <c r="AE11" s="67"/>
-      <c r="AF11" s="67"/>
-      <c r="AG11" s="69"/>
-      <c r="AH11" s="70"/>
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="52"/>
+      <c r="AH11" s="48"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="5"/>
     </row>
@@ -2077,7 +2036,7 @@
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="26" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="2"/>
@@ -2088,36 +2047,36 @@
       <c r="H12" s="5"/>
       <c r="I12" s="2"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
       <c r="M12" s="2"/>
       <c r="N12" s="5"/>
       <c r="O12" s="2"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="59"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="52"/>
       <c r="U12" s="2"/>
       <c r="V12" s="5"/>
       <c r="W12" s="2"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="5"/>
-      <c r="AA12" s="59"/>
-      <c r="AB12" s="59"/>
+      <c r="AA12" s="52"/>
+      <c r="AB12" s="52"/>
       <c r="AC12" s="17"/>
       <c r="AD12" s="20"/>
       <c r="AE12" s="17"/>
       <c r="AF12" s="21"/>
-      <c r="AG12" s="41"/>
-      <c r="AH12" s="42"/>
+      <c r="AG12" s="23"/>
+      <c r="AH12" s="24"/>
       <c r="AI12" s="22"/>
       <c r="AJ12" s="19"/>
     </row>
     <row r="13" spans="1:36" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="2"/>
@@ -2128,42 +2087,37 @@
       <c r="H13" s="5"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="6"/>
-      <c r="Q13" s="53"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="52"/>
+      <c r="T13" s="52"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="5"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
+      <c r="AA13" s="52"/>
+      <c r="AB13" s="52"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="5"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="5"/>
       <c r="AG13" s="17"/>
       <c r="AH13" s="21"/>
-      <c r="AI13" s="41"/>
-      <c r="AJ13" s="42"/>
+      <c r="AI13" s="23"/>
+      <c r="AJ13" s="24"/>
     </row>
     <row r="14" spans="1:36" ht="13" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AH2"/>
@@ -2179,6 +2133,11 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.39374999999999999" bottom="0.39374999999999999" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2193,1388 +2152,1404 @@
   </sheetPr>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" style="36" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" style="36" customWidth="1"/>
-    <col min="3" max="3" width="88.1796875" style="36" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" style="36" customWidth="1"/>
-    <col min="5" max="6" width="10.1796875" style="36" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" style="36" customWidth="1"/>
-    <col min="8" max="16384" width="11.54296875" style="36"/>
+    <col min="1" max="1" width="5.08984375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" style="34" customWidth="1"/>
+    <col min="3" max="3" width="88.1796875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" style="34" customWidth="1"/>
+    <col min="5" max="6" width="10.1796875" style="34" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" style="34" customWidth="1"/>
+    <col min="8" max="16384" width="11.54296875" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
+      <c r="A3" s="35">
         <v>1</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="36">
         <v>44950</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38">
+      <c r="D3" s="35"/>
+      <c r="E3" s="36">
         <v>44950</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="36">
         <v>44950</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
+      <c r="A4" s="35">
         <v>2</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="36">
         <f>B3</f>
         <v>44950</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38">
+      <c r="D4" s="35"/>
+      <c r="E4" s="36">
         <f>E3</f>
         <v>44950</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="36">
         <f>F3</f>
         <v>44950</v>
       </c>
-      <c r="G4" s="40" t="str">
+      <c r="G4" s="38" t="str">
         <f>G3</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="35" t="s">
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
+      <c r="A6" s="35">
         <v>3</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="36">
         <f>B4</f>
         <v>44950</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38">
+      <c r="D6" s="35"/>
+      <c r="E6" s="36">
         <f>E4</f>
         <v>44950</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="36">
         <f>F4</f>
         <v>44950</v>
       </c>
-      <c r="G6" s="40" t="str">
+      <c r="G6" s="38" t="str">
         <f>G4</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
+      <c r="A7" s="35">
         <v>4</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="36">
         <f>B6</f>
         <v>44950</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="38">
+      <c r="D7" s="35"/>
+      <c r="E7" s="36">
         <f>E6</f>
         <v>44950</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="36">
         <f t="shared" ref="F7:G9" si="0">F6</f>
         <v>44950</v>
       </c>
-      <c r="G7" s="40" t="str">
+      <c r="G7" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37">
+      <c r="A8" s="35">
         <v>5</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="36">
         <f>B7</f>
         <v>44950</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38">
+      <c r="D8" s="35"/>
+      <c r="E8" s="36">
         <f>E7</f>
         <v>44950</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="36">
         <f t="shared" si="0"/>
         <v>44950</v>
       </c>
-      <c r="G8" s="40" t="str">
+      <c r="G8" s="38" t="str">
         <f t="shared" si="0"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="A9" s="35">
         <v>6</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="36">
         <f>B6</f>
         <v>44950</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38">
+      <c r="D9" s="35"/>
+      <c r="E9" s="36">
         <f>E8</f>
         <v>44950</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="36">
         <f t="shared" si="0"/>
         <v>44950</v>
       </c>
-      <c r="G9" s="40" t="str">
+      <c r="G9" s="38" t="str">
         <f>G8</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="35" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37">
+      <c r="A11" s="35">
         <v>7</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="36">
         <v>44957</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38">
+      <c r="D11" s="35"/>
+      <c r="E11" s="36">
         <v>44957</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="36">
         <f>E11</f>
         <v>44957</v>
       </c>
-      <c r="G11" s="40" t="str">
+      <c r="G11" s="38" t="str">
         <f>G9</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37">
+      <c r="A12" s="35">
         <f>A11+1</f>
         <v>8</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="36">
         <f>B11</f>
         <v>44957</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38">
+      <c r="D12" s="35"/>
+      <c r="E12" s="36">
         <f>E11</f>
         <v>44957</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="36">
         <f t="shared" ref="F12:G20" si="1">F11</f>
         <v>44957</v>
       </c>
-      <c r="G12" s="40" t="str">
+      <c r="G12" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37">
+      <c r="A13" s="35">
         <f>A12+1</f>
         <v>9</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="36">
         <f>B12</f>
         <v>44957</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38">
+      <c r="D13" s="35"/>
+      <c r="E13" s="36">
         <f>E12</f>
         <v>44957</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="36">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G13" s="40" t="str">
+      <c r="G13" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37">
+      <c r="A14" s="35">
         <f t="shared" ref="A14:A20" si="2">A13+1</f>
         <v>10</v>
       </c>
-      <c r="B14" s="38">
+      <c r="B14" s="36">
         <f t="shared" ref="B14:B20" si="3">B13</f>
         <v>44957</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38">
+      <c r="D14" s="35"/>
+      <c r="E14" s="36">
         <f t="shared" ref="E14:E20" si="4">E13</f>
         <v>44957</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="36">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G14" s="40" t="str">
+      <c r="G14" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="35" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37">
+      <c r="A16" s="35">
         <f>A14+1</f>
         <v>11</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="36">
         <f>B14</f>
         <v>44957</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38">
+      <c r="D16" s="35"/>
+      <c r="E16" s="36">
         <f>E14</f>
         <v>44957</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="36">
         <f>F14</f>
         <v>44957</v>
       </c>
-      <c r="G16" s="40" t="str">
+      <c r="G16" s="38" t="str">
         <f>G14</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37">
+      <c r="A17" s="35">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="36">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38">
+      <c r="D17" s="35"/>
+      <c r="E17" s="36">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="36">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G17" s="40" t="str">
+      <c r="G17" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37">
+      <c r="A18" s="35">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B18" s="38">
+      <c r="B18" s="36">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38">
+      <c r="D18" s="35"/>
+      <c r="E18" s="36">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="36">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G18" s="40" t="str">
+      <c r="G18" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37">
+      <c r="A19" s="35">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="36">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38">
+      <c r="D19" s="35"/>
+      <c r="E19" s="36">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="36">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G19" s="40" t="str">
+      <c r="G19" s="38" t="str">
         <f t="shared" si="1"/>
         <v>Terminer</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37">
+      <c r="A20" s="35">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B20" s="38">
+      <c r="B20" s="36">
         <f t="shared" si="3"/>
         <v>44957</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38">
+      <c r="D20" s="35"/>
+      <c r="E20" s="36">
         <f t="shared" si="4"/>
         <v>44957</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="36">
         <f t="shared" si="1"/>
         <v>44957</v>
       </c>
-      <c r="G20" s="40" t="str">
+      <c r="G20" s="38" t="str">
         <f>G19</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="35" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37">
+      <c r="A22" s="35">
         <f>A20+1</f>
         <v>16</v>
       </c>
-      <c r="B22" s="38">
+      <c r="B22" s="36">
         <v>44964</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38">
+      <c r="D22" s="35"/>
+      <c r="E22" s="36">
         <f>B22</f>
         <v>44964</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="36">
         <f>E22</f>
         <v>44964</v>
       </c>
-      <c r="G22" s="40" t="str">
+      <c r="G22" s="38" t="str">
         <f>G20</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37">
+      <c r="A23" s="35">
         <f>A22+1</f>
         <v>17</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="36">
         <f>B22</f>
         <v>44964</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38">
+      <c r="D23" s="35"/>
+      <c r="E23" s="36">
         <f>B23</f>
         <v>44964</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="36">
         <f>E23</f>
         <v>44964</v>
       </c>
-      <c r="G23" s="40" t="str">
+      <c r="G23" s="38" t="str">
         <f>G22</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37">
+      <c r="A24" s="35">
         <f>A23+1</f>
         <v>18</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="36">
         <f>B23</f>
         <v>44964</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="38">
+      <c r="D24" s="35"/>
+      <c r="E24" s="36">
         <f>B24</f>
         <v>44964</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="36">
         <f>E24</f>
         <v>44964</v>
       </c>
-      <c r="G24" s="40" t="str">
+      <c r="G24" s="38" t="str">
         <f>G22</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37">
+      <c r="A25" s="35">
         <f>A24+1</f>
         <v>19</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="36">
         <f>B24</f>
         <v>44964</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="38">
+      <c r="D25" s="35"/>
+      <c r="E25" s="36">
         <f>B25</f>
         <v>44964</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="36">
         <f>E25</f>
         <v>44964</v>
       </c>
-      <c r="G25" s="40" t="str">
+      <c r="G25" s="38" t="str">
         <f>G23</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="35" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37">
+      <c r="A27" s="35">
         <f>A25+1</f>
         <v>20</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="36">
         <f>B25</f>
         <v>44964</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38">
+      <c r="D27" s="35"/>
+      <c r="E27" s="36">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="36">
         <f t="shared" ref="F27:F32" si="5">E27</f>
         <v>44964</v>
       </c>
-      <c r="G27" s="40" t="str">
+      <c r="G27" s="38" t="str">
         <f>G25</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37">
+      <c r="A28" s="35">
         <f t="shared" ref="A28:A32" si="6">A27+1</f>
         <v>21</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B28" s="36">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="38">
+      <c r="D28" s="35"/>
+      <c r="E28" s="36">
         <v>44978</v>
       </c>
-      <c r="F28" s="38">
+      <c r="F28" s="36">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G28" s="40" t="str">
+      <c r="G28" s="38" t="str">
         <f>G27</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37">
+      <c r="A29" s="35">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="36">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="38">
+      <c r="D29" s="35"/>
+      <c r="E29" s="36">
         <f>E28</f>
         <v>44978</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="36">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G29" s="40" t="str">
+      <c r="G29" s="38" t="str">
         <f>G28</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="48.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37">
+      <c r="A30" s="35">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="36">
         <f>B27</f>
         <v>44964</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="36">
         <f>E29</f>
         <v>44978</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="36">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G30" s="40" t="str">
+      <c r="G30" s="38" t="str">
         <f>G29</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37">
+      <c r="A31" s="35">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B31" s="36">
         <f>B29</f>
         <v>44964</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="38">
+      <c r="D31" s="35"/>
+      <c r="E31" s="36">
         <f>E30</f>
         <v>44978</v>
       </c>
-      <c r="F31" s="38">
+      <c r="F31" s="36">
         <f t="shared" si="5"/>
         <v>44978</v>
       </c>
-      <c r="G31" s="40" t="str">
+      <c r="G31" s="38" t="str">
         <f>G30</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37">
+      <c r="A32" s="35">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="B32" s="38">
+      <c r="B32" s="36">
         <v>44985</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="38">
+      <c r="D32" s="35"/>
+      <c r="E32" s="36">
         <f>B32</f>
         <v>44985</v>
       </c>
-      <c r="F32" s="38">
+      <c r="F32" s="36">
         <f t="shared" si="5"/>
         <v>44985</v>
       </c>
-      <c r="G32" s="40" t="str">
+      <c r="G32" s="38" t="str">
         <f>G31</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="35" t="s">
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
     </row>
     <row r="34" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37">
+      <c r="A34" s="35">
         <f>A32+1</f>
         <v>26</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34" s="36">
         <f>E28</f>
         <v>44978</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38">
+      <c r="D34" s="35"/>
+      <c r="E34" s="36">
         <f>E31</f>
         <v>44978</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="36">
         <f>E34</f>
         <v>44978</v>
       </c>
-      <c r="G34" s="40" t="str">
+      <c r="G34" s="38" t="str">
         <f>G30</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37">
+      <c r="A35" s="35">
         <f>A34+1</f>
         <v>27</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="36">
         <f>B34</f>
         <v>44978</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38">
+      <c r="D35" s="35"/>
+      <c r="E35" s="36">
         <f>E34</f>
         <v>44978</v>
       </c>
-      <c r="F35" s="38">
+      <c r="F35" s="36">
         <f>E35</f>
         <v>44978</v>
       </c>
-      <c r="G35" s="39" t="str">
+      <c r="G35" s="37" t="str">
         <f>G34</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
+      <c r="A36" s="35">
         <f>A35+1</f>
         <v>28</v>
       </c>
-      <c r="B36" s="38">
+      <c r="B36" s="36">
         <f>B35</f>
         <v>44978</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="38">
+      <c r="D36" s="35"/>
+      <c r="E36" s="36">
         <f>E35</f>
         <v>44978</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="36">
         <f>E36</f>
         <v>44978</v>
       </c>
-      <c r="G36" s="39" t="str">
+      <c r="G36" s="37" t="str">
         <f>G35</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="35" t="s">
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
     </row>
     <row r="38" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37">
+      <c r="A38" s="35">
         <f>A36+1</f>
         <v>29</v>
       </c>
-      <c r="B38" s="38">
+      <c r="B38" s="36">
         <v>44985</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38">
+      <c r="D38" s="35"/>
+      <c r="E38" s="36">
         <f>B38</f>
         <v>44985</v>
       </c>
-      <c r="F38" s="38">
+      <c r="F38" s="36">
         <f>E38</f>
         <v>44985</v>
       </c>
-      <c r="G38" s="39" t="str">
+      <c r="G38" s="37" t="str">
         <f>G36</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37">
+      <c r="A39" s="35">
         <f>A38+1</f>
         <v>30</v>
       </c>
-      <c r="B39" s="38">
+      <c r="B39" s="36">
         <f>B38</f>
         <v>44985</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="37"/>
-      <c r="E39" s="38">
+      <c r="D39" s="35"/>
+      <c r="E39" s="36">
         <f>B39</f>
         <v>44985</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="36">
         <f>E39</f>
         <v>44985</v>
       </c>
-      <c r="G39" s="39" t="str">
+      <c r="G39" s="37" t="str">
         <f>G38</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37">
+      <c r="A40" s="35">
         <f>A39+1</f>
         <v>31</v>
       </c>
-      <c r="B40" s="38">
+      <c r="B40" s="36">
         <f>B39</f>
         <v>44985</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="37"/>
-      <c r="E40" s="38">
+      <c r="D40" s="35"/>
+      <c r="E40" s="36">
         <f>B40</f>
         <v>44985</v>
       </c>
-      <c r="F40" s="38">
+      <c r="F40" s="36">
         <f>E40</f>
         <v>44985</v>
       </c>
-      <c r="G40" s="39" t="str">
+      <c r="G40" s="37" t="str">
         <f>G39</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="35" t="s">
+      <c r="A41" s="35"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="37"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
     </row>
     <row r="42" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37">
+      <c r="A42" s="35">
         <f>A40+1</f>
         <v>32</v>
       </c>
-      <c r="B42" s="38">
+      <c r="B42" s="36">
         <f>B40</f>
         <v>44985</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="37"/>
-      <c r="E42" s="38">
+      <c r="D42" s="35"/>
+      <c r="E42" s="36">
         <v>44992</v>
       </c>
-      <c r="F42" s="38">
+      <c r="F42" s="36">
         <v>45006</v>
       </c>
-      <c r="G42" s="39" t="str">
+      <c r="G42" s="37" t="str">
         <f>G40</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37">
+      <c r="A43" s="35">
         <f>A42+1</f>
         <v>33</v>
       </c>
-      <c r="B43" s="38">
+      <c r="B43" s="36">
         <f>B42</f>
         <v>44985</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="37"/>
-      <c r="E43" s="38">
+      <c r="D43" s="35"/>
+      <c r="E43" s="36">
         <f>E42</f>
         <v>44992</v>
       </c>
-      <c r="F43" s="38">
+      <c r="F43" s="36">
         <f>+F42</f>
         <v>45006</v>
       </c>
-      <c r="G43" s="39" t="str">
+      <c r="G43" s="37" t="str">
         <f>G42</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37">
+      <c r="A44" s="35">
         <f>A43+1</f>
         <v>34</v>
       </c>
-      <c r="B44" s="38">
+      <c r="B44" s="36">
         <f>B43</f>
         <v>44985</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="37"/>
-      <c r="E44" s="38">
+      <c r="D44" s="35"/>
+      <c r="E44" s="36">
         <f>E43</f>
         <v>44992</v>
       </c>
-      <c r="F44" s="38">
+      <c r="F44" s="36">
         <f>+F43</f>
         <v>45006</v>
       </c>
-      <c r="G44" s="39" t="str">
+      <c r="G44" s="37" t="str">
         <f>G42</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37">
+      <c r="A45" s="35">
         <f>A44+1</f>
         <v>35</v>
       </c>
-      <c r="B45" s="38">
+      <c r="B45" s="36">
         <f>B44</f>
         <v>44985</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="37"/>
-      <c r="E45" s="38">
+      <c r="D45" s="35"/>
+      <c r="E45" s="36">
         <f>E44</f>
         <v>44992</v>
       </c>
-      <c r="F45" s="38">
+      <c r="F45" s="36">
         <v>45013</v>
       </c>
-      <c r="G45" s="39" t="str">
+      <c r="G45" s="37" t="str">
         <f>G44</f>
         <v>Terminer</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="35" t="s">
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
     </row>
     <row r="47" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="37">
+      <c r="A47" s="35">
         <f>A45+1</f>
         <v>36</v>
       </c>
-      <c r="B47" s="38">
+      <c r="B47" s="36">
         <f>B45</f>
         <v>44985</v>
       </c>
-      <c r="C47" s="37" t="s">
+      <c r="C47" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="D47" s="37"/>
-      <c r="E47" s="38">
+      <c r="D47" s="35"/>
+      <c r="E47" s="36">
         <v>45020</v>
       </c>
-      <c r="F47" s="38">
+      <c r="F47" s="36">
         <f>F48</f>
         <v>45034</v>
       </c>
-      <c r="G47" s="39" t="s">
+      <c r="G47" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="37">
+      <c r="A48" s="35">
         <f t="shared" ref="A48:A52" si="7">A47+1</f>
         <v>37</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="36">
         <f t="shared" ref="B48:B52" si="8">B47</f>
         <v>44985</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D48" s="37"/>
-      <c r="E48" s="38">
+      <c r="D48" s="35"/>
+      <c r="E48" s="36">
         <f t="shared" ref="E48:E52" si="9">E47</f>
         <v>45020</v>
       </c>
-      <c r="F48" s="38">
+      <c r="F48" s="36">
         <v>45034</v>
       </c>
-      <c r="G48" s="39" t="s">
+      <c r="G48" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37">
+      <c r="A49" s="35">
         <f t="shared" si="7"/>
         <v>38</v>
       </c>
-      <c r="B49" s="38">
+      <c r="B49" s="36">
         <f t="shared" si="8"/>
         <v>44985</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C49" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="37"/>
-      <c r="E49" s="38">
+      <c r="D49" s="35"/>
+      <c r="E49" s="36">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F49" s="37"/>
-      <c r="G49" s="45" t="s">
-        <v>125</v>
+      <c r="F49" s="36">
+        <v>45050</v>
+      </c>
+      <c r="G49" s="37" t="str">
+        <f>G48</f>
+        <v>Terminer</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="37">
+      <c r="A50" s="35">
         <f t="shared" si="7"/>
         <v>39</v>
       </c>
-      <c r="B50" s="38">
+      <c r="B50" s="36">
         <f t="shared" si="8"/>
         <v>44985</v>
       </c>
-      <c r="C50" s="37" t="s">
+      <c r="C50" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="37"/>
-      <c r="E50" s="38">
+      <c r="D50" s="35"/>
+      <c r="E50" s="36">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F50" s="38">
+      <c r="F50" s="36">
         <f>F48</f>
         <v>45034</v>
       </c>
-      <c r="G50" s="39" t="s">
+      <c r="G50" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="37">
+      <c r="A51" s="35">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
-      <c r="B51" s="38">
+      <c r="B51" s="36">
         <f t="shared" si="8"/>
         <v>44985</v>
       </c>
-      <c r="C51" s="37" t="s">
+      <c r="C51" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="D51" s="37"/>
-      <c r="E51" s="38">
+      <c r="D51" s="35"/>
+      <c r="E51" s="36">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F51" s="38">
+      <c r="F51" s="36">
         <f>F50</f>
         <v>45034</v>
       </c>
-      <c r="G51" s="39" t="s">
+      <c r="G51" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="37">
+      <c r="A52" s="35">
         <f t="shared" si="7"/>
         <v>41</v>
       </c>
-      <c r="B52" s="38">
+      <c r="B52" s="36">
         <f t="shared" si="8"/>
         <v>44985</v>
       </c>
-      <c r="C52" s="37" t="s">
+      <c r="C52" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="37"/>
-      <c r="E52" s="38">
+      <c r="D52" s="35"/>
+      <c r="E52" s="36">
         <f t="shared" si="9"/>
         <v>45020</v>
       </c>
-      <c r="F52" s="38">
+      <c r="F52" s="36">
         <f>F51</f>
         <v>45034</v>
       </c>
-      <c r="G52" s="39" t="s">
+      <c r="G52" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="55"/>
-      <c r="B53" s="55"/>
-      <c r="C53" s="56" t="s">
+      <c r="A53" s="45"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="57"/>
-      <c r="G53" s="57"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
     </row>
     <row r="54" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="37">
+      <c r="A54" s="35">
         <f>A52+1</f>
         <v>42</v>
       </c>
-      <c r="B54" s="38">
+      <c r="B54" s="36">
         <v>45034</v>
       </c>
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="38">
+      <c r="D54" s="35"/>
+      <c r="E54" s="36">
         <v>45048</v>
       </c>
-      <c r="F54" s="37"/>
-      <c r="G54" s="45" t="s">
-        <v>126</v>
+      <c r="F54" s="36">
+        <f>E54</f>
+        <v>45048</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="71.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="34" t="s">
+      <c r="A55" s="35"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
     </row>
     <row r="56" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="37">
+      <c r="A56" s="35">
         <f>A54+1</f>
         <v>43</v>
       </c>
-      <c r="B56" s="38">
+      <c r="B56" s="36">
         <f>+B54</f>
         <v>45034</v>
       </c>
-      <c r="C56" s="37" t="s">
+      <c r="C56" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="D56" s="37"/>
-      <c r="E56" s="38">
+      <c r="D56" s="35"/>
+      <c r="E56" s="36">
         <v>45048</v>
       </c>
-      <c r="F56" s="38">
+      <c r="F56" s="36">
         <v>45041</v>
       </c>
-      <c r="G56" s="39" t="s">
+      <c r="G56" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="37">
+      <c r="A57" s="35">
         <f>A56+1</f>
         <v>44</v>
       </c>
-      <c r="B57" s="38">
+      <c r="B57" s="36">
         <f>B56</f>
         <v>45034</v>
       </c>
-      <c r="C57" s="37" t="s">
+      <c r="C57" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="D57" s="37"/>
-      <c r="E57" s="38">
+      <c r="D57" s="35"/>
+      <c r="E57" s="36">
         <v>45048</v>
       </c>
-      <c r="F57" s="38">
+      <c r="F57" s="36">
         <f>F56</f>
         <v>45041</v>
       </c>
-      <c r="G57" s="39" t="s">
+      <c r="G57" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="37">
+      <c r="A58" s="35">
         <f>A57+1</f>
         <v>45</v>
       </c>
-      <c r="B58" s="38">
+      <c r="B58" s="36">
         <f>B57</f>
         <v>45034</v>
       </c>
-      <c r="C58" s="37" t="s">
+      <c r="C58" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="D58" s="37"/>
-      <c r="E58" s="38">
+      <c r="D58" s="35"/>
+      <c r="E58" s="36">
         <v>45048</v>
       </c>
-      <c r="F58" s="38">
+      <c r="F58" s="36">
         <f>F57</f>
         <v>45041</v>
       </c>
-      <c r="G58" s="39" t="s">
+      <c r="G58" s="37" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="34" t="s">
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
     </row>
     <row r="60" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="37">
+      <c r="A60" s="35">
         <f>A58+1</f>
         <v>46</v>
       </c>
-      <c r="B60" s="38">
+      <c r="B60" s="36">
         <f>B58</f>
         <v>45034</v>
       </c>
-      <c r="C60" s="37" t="s">
+      <c r="C60" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="E60" s="38">
+      <c r="E60" s="36">
         <v>45048</v>
       </c>
-      <c r="F60" s="37"/>
-      <c r="G60" s="45" t="s">
-        <v>125</v>
+      <c r="F60" s="36">
+        <f>E60</f>
+        <v>45048</v>
+      </c>
+      <c r="G60" s="37" t="str">
+        <f>G58</f>
+        <v>Terminer</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="37">
+      <c r="A61" s="35">
         <f>A60+1</f>
         <v>47</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="36">
         <f>B60</f>
         <v>45034</v>
       </c>
-      <c r="C61" s="37" t="s">
+      <c r="C61" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="D61" s="37"/>
-      <c r="E61" s="38">
+      <c r="D61" s="35"/>
+      <c r="E61" s="36">
         <v>45048</v>
       </c>
-      <c r="F61" s="37"/>
-      <c r="G61" s="45" t="str">
+      <c r="F61" s="36">
+        <f t="shared" ref="F61:F62" si="10">E61</f>
+        <v>45048</v>
+      </c>
+      <c r="G61" s="37" t="str">
         <f>G60</f>
-        <v>Commencer</v>
+        <v>Terminer</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="37">
+      <c r="A62" s="35">
         <f>A61+1</f>
         <v>48</v>
       </c>
-      <c r="B62" s="38">
+      <c r="B62" s="36">
         <f>B61</f>
         <v>45034</v>
       </c>
-      <c r="C62" s="37" t="s">
+      <c r="C62" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="D62" s="37"/>
-      <c r="E62" s="38">
+      <c r="D62" s="35"/>
+      <c r="E62" s="36">
         <v>45048</v>
       </c>
-      <c r="F62" s="37"/>
-      <c r="G62" s="45" t="str">
+      <c r="F62" s="36">
+        <f t="shared" si="10"/>
+        <v>45048</v>
+      </c>
+      <c r="G62" s="37" t="str">
         <f>G61</f>
-        <v>Commencer</v>
+        <v>Terminer</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44"/>
-      <c r="B63" s="44"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3605,74 +3580,74 @@
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="62"/>
-      <c r="G3" s="60" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="60"/>
-      <c r="I3" s="58" t="s">
+      <c r="H3" s="49"/>
+      <c r="I3" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58" t="s">
+      <c r="J3" s="51"/>
+      <c r="K3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="58"/>
-      <c r="M3" s="60" t="s">
+      <c r="L3" s="51"/>
+      <c r="M3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60" t="s">
+      <c r="N3" s="49"/>
+      <c r="O3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60" t="s">
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="60"/>
-      <c r="S3" s="60" t="s">
+      <c r="R3" s="49"/>
+      <c r="S3" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="60"/>
-      <c r="U3" s="58" t="s">
+      <c r="T3" s="49"/>
+      <c r="U3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="V3" s="58"/>
-      <c r="W3" s="60" t="s">
+      <c r="V3" s="51"/>
+      <c r="W3" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="58" t="s">
+      <c r="X3" s="49"/>
+      <c r="Y3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="60" t="s">
+      <c r="Z3" s="51"/>
+      <c r="AA3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="AB3" s="60"/>
-      <c r="AC3" s="58" t="s">
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58" t="s">
+      <c r="AD3" s="51"/>
+      <c r="AE3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58" t="s">
+      <c r="AF3" s="51"/>
+      <c r="AG3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="58" t="s">
+      <c r="AH3" s="51"/>
+      <c r="AI3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AJ3" s="58"/>
+      <c r="AJ3" s="51"/>
     </row>
     <row r="4" spans="1:36" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -3689,30 +3664,30 @@
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="59"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="2"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="5"/>
-      <c r="S4" s="59" t="s">
+      <c r="S4" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="59"/>
+      <c r="T4" s="52"/>
       <c r="U4" s="2"/>
       <c r="V4" s="5"/>
       <c r="W4" s="2"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-      <c r="AA4" s="59" t="s">
+      <c r="AA4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" s="59"/>
+      <c r="AB4" s="52"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="2"/>
@@ -3737,24 +3712,24 @@
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
       <c r="M5" s="2"/>
       <c r="N5" s="5"/>
       <c r="O5" s="2"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
       <c r="U5" s="2"/>
       <c r="V5" s="5"/>
       <c r="W5" s="2"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-      <c r="AA5" s="59"/>
-      <c r="AB5" s="59"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="52"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="5"/>
       <c r="AE5" s="2"/>
@@ -3779,24 +3754,24 @@
       <c r="H6" s="10"/>
       <c r="I6" s="11"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="2"/>
       <c r="N6" s="5"/>
       <c r="O6" s="2"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="52"/>
       <c r="U6" s="2"/>
       <c r="V6" s="5"/>
       <c r="W6" s="2"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="5"/>
       <c r="AE6" s="2"/>
@@ -3821,24 +3796,24 @@
       <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
       <c r="M7" s="2"/>
       <c r="N7" s="5"/>
       <c r="O7" s="2"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="5"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52"/>
       <c r="U7" s="2"/>
       <c r="V7" s="5"/>
       <c r="W7" s="2"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="59"/>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="52"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="5"/>
       <c r="AE7" s="2"/>
@@ -3863,24 +3838,24 @@
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="9"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="5"/>
-      <c r="S8" s="59"/>
-      <c r="T8" s="59"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
       <c r="U8" s="2"/>
       <c r="V8" s="5"/>
       <c r="W8" s="2"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="59"/>
-      <c r="AB8" s="59"/>
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="52"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="5"/>
       <c r="AE8" s="2"/>
@@ -3905,24 +3880,24 @@
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="2"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="9"/>
       <c r="R9" s="12"/>
-      <c r="S9" s="59"/>
-      <c r="T9" s="59"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
       <c r="U9" s="13"/>
       <c r="V9" s="11"/>
       <c r="W9" s="2"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-      <c r="AA9" s="59"/>
-      <c r="AB9" s="59"/>
+      <c r="AA9" s="52"/>
+      <c r="AB9" s="52"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="5"/>
       <c r="AE9" s="2"/>
@@ -3947,24 +3922,24 @@
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
       <c r="M10" s="2"/>
       <c r="N10" s="5"/>
       <c r="O10" s="2"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
+      <c r="S10" s="52"/>
+      <c r="T10" s="52"/>
       <c r="U10" s="2"/>
       <c r="V10" s="5"/>
       <c r="W10" s="9"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="13"/>
       <c r="Z10" s="11"/>
-      <c r="AA10" s="59"/>
-      <c r="AB10" s="59"/>
+      <c r="AA10" s="52"/>
+      <c r="AB10" s="52"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="5"/>
       <c r="AE10" s="2"/>
@@ -3989,24 +3964,24 @@
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
       <c r="M11" s="2"/>
       <c r="N11" s="5"/>
       <c r="O11" s="2"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="52"/>
       <c r="U11" s="2"/>
       <c r="V11" s="5"/>
       <c r="W11" s="2"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="5"/>
-      <c r="AA11" s="59"/>
-      <c r="AB11" s="59"/>
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="52"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="11"/>
       <c r="AE11" s="2"/>
@@ -4029,24 +4004,24 @@
       <c r="H12" s="12"/>
       <c r="I12" s="13"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
       <c r="M12" s="13"/>
       <c r="N12" s="12"/>
       <c r="O12" s="13"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13"/>
       <c r="R12" s="12"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="59"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="52"/>
       <c r="U12" s="13"/>
       <c r="V12" s="10"/>
       <c r="W12" s="13"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="11"/>
-      <c r="AA12" s="59"/>
-      <c r="AB12" s="59"/>
+      <c r="AA12" s="52"/>
+      <c r="AB12" s="52"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="5"/>
       <c r="AE12" s="2"/>
@@ -4069,24 +4044,24 @@
       <c r="H13" s="6"/>
       <c r="I13" s="2"/>
       <c r="J13" s="5"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
       <c r="M13" s="2"/>
       <c r="N13" s="5"/>
       <c r="O13" s="2"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="59"/>
-      <c r="T13" s="59"/>
+      <c r="S13" s="52"/>
+      <c r="T13" s="52"/>
       <c r="U13" s="2"/>
       <c r="V13" s="5"/>
       <c r="W13" s="2"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="59"/>
+      <c r="AA13" s="52"/>
+      <c r="AB13" s="52"/>
       <c r="AC13" s="9"/>
       <c r="AD13" s="11"/>
       <c r="AE13" s="2"/>
@@ -4109,24 +4084,24 @@
       <c r="H14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="59"/>
-      <c r="T14" s="59"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="52"/>
       <c r="U14" s="2"/>
       <c r="V14" s="5"/>
       <c r="W14" s="2"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-      <c r="AA14" s="59"/>
-      <c r="AB14" s="59"/>
+      <c r="AA14" s="52"/>
+      <c r="AB14" s="52"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="5"/>
       <c r="AE14" s="9"/>
@@ -4140,11 +4115,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="20">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AE3:AF3"/>
     <mergeCell ref="AG3:AH3"/>
@@ -4160,6 +4130,11 @@
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.39374999999999999" bottom="0.39374999999999999" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>